<commit_message>
fix(form): fix missing node error
</commit_message>
<xml_diff>
--- a/forms/app/register.xlsx
+++ b/forms/app/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Work/dccms/daily-register/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC66D03-B687-9E4A-9950-26CC49A01284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E1470B-9180-3A42-8B2C-A7991559C697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="184">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -584,6 +584,18 @@
   </si>
   <si>
     <t>Time of observation</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -2432,10 +2444,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV1045"/>
+  <dimension ref="A1:IV1046"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2776,37 +2788,41 @@
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="64" t="s">
-        <v>21</v>
+        <v>183</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>41</v>
+        <v>180</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>42</v>
+        <v>181</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68" t="s">
+        <v>25</v>
+      </c>
       <c r="G3" s="68"/>
       <c r="H3" s="68"/>
       <c r="I3" s="68"/>
       <c r="J3" s="68"/>
-      <c r="K3" s="69"/>
+      <c r="K3" s="69" t="s">
+        <v>182</v>
+      </c>
       <c r="L3" s="69"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
-      <c r="Y3" s="73"/>
-      <c r="Z3" s="73"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="71"/>
       <c r="AA3"/>
       <c r="AB3"/>
       <c r="AC3"/>
@@ -3040,13 +3056,13 @@
     </row>
     <row r="4" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="64" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D4" s="69"/>
       <c r="E4" s="68"/>
@@ -3307,10 +3323,10 @@
         <v>25</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="69"/>
       <c r="E5" s="68"/>
@@ -3568,10 +3584,14 @@
     </row>
     <row r="6" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="64" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="75"/>
+      <c r="B6" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>51</v>
+      </c>
       <c r="D6" s="69"/>
       <c r="E6" s="68"/>
       <c r="F6" s="68"/>
@@ -4087,58 +4107,278 @@
       <c r="IV7"/>
     </row>
     <row r="8" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="25"/>
+      <c r="A8" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="74"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="73"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="73"/>
+      <c r="V8" s="73"/>
+      <c r="W8" s="73"/>
+      <c r="X8" s="73"/>
+      <c r="Y8" s="73"/>
+      <c r="Z8" s="73"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+      <c r="AO8"/>
+      <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8"/>
+      <c r="AS8"/>
+      <c r="AT8"/>
+      <c r="AU8"/>
+      <c r="AV8"/>
+      <c r="AW8"/>
+      <c r="AX8"/>
+      <c r="AY8"/>
+      <c r="AZ8"/>
+      <c r="BA8"/>
+      <c r="BB8"/>
+      <c r="BC8"/>
+      <c r="BD8"/>
+      <c r="BE8"/>
+      <c r="BF8"/>
+      <c r="BG8"/>
+      <c r="BH8"/>
+      <c r="BI8"/>
+      <c r="BJ8"/>
+      <c r="BK8"/>
+      <c r="BL8"/>
+      <c r="BM8"/>
+      <c r="BN8"/>
+      <c r="BO8"/>
+      <c r="BP8"/>
+      <c r="BQ8"/>
+      <c r="BR8"/>
+      <c r="BS8"/>
+      <c r="BT8"/>
+      <c r="BU8"/>
+      <c r="BV8"/>
+      <c r="BW8"/>
+      <c r="BX8"/>
+      <c r="BY8"/>
+      <c r="BZ8"/>
+      <c r="CA8"/>
+      <c r="CB8"/>
+      <c r="CC8"/>
+      <c r="CD8"/>
+      <c r="CE8"/>
+      <c r="CF8"/>
+      <c r="CG8"/>
+      <c r="CH8"/>
+      <c r="CI8"/>
+      <c r="CJ8"/>
+      <c r="CK8"/>
+      <c r="CL8"/>
+      <c r="CM8"/>
+      <c r="CN8"/>
+      <c r="CO8"/>
+      <c r="CP8"/>
+      <c r="CQ8"/>
+      <c r="CR8"/>
+      <c r="CS8"/>
+      <c r="CT8"/>
+      <c r="CU8"/>
+      <c r="CV8"/>
+      <c r="CW8"/>
+      <c r="CX8"/>
+      <c r="CY8"/>
+      <c r="CZ8"/>
+      <c r="DA8"/>
+      <c r="DB8"/>
+      <c r="DC8"/>
+      <c r="DD8"/>
+      <c r="DE8"/>
+      <c r="DF8"/>
+      <c r="DG8"/>
+      <c r="DH8"/>
+      <c r="DI8"/>
+      <c r="DJ8"/>
+      <c r="DK8"/>
+      <c r="DL8"/>
+      <c r="DM8"/>
+      <c r="DN8"/>
+      <c r="DO8"/>
+      <c r="DP8"/>
+      <c r="DQ8"/>
+      <c r="DR8"/>
+      <c r="DS8"/>
+      <c r="DT8"/>
+      <c r="DU8"/>
+      <c r="DV8"/>
+      <c r="DW8"/>
+      <c r="DX8"/>
+      <c r="DY8"/>
+      <c r="DZ8"/>
+      <c r="EA8"/>
+      <c r="EB8"/>
+      <c r="EC8"/>
+      <c r="ED8"/>
+      <c r="EE8"/>
+      <c r="EF8"/>
+      <c r="EG8"/>
+      <c r="EH8"/>
+      <c r="EI8"/>
+      <c r="EJ8"/>
+      <c r="EK8"/>
+      <c r="EL8"/>
+      <c r="EM8"/>
+      <c r="EN8"/>
+      <c r="EO8"/>
+      <c r="EP8"/>
+      <c r="EQ8"/>
+      <c r="ER8"/>
+      <c r="ES8"/>
+      <c r="ET8"/>
+      <c r="EU8"/>
+      <c r="EV8"/>
+      <c r="EW8"/>
+      <c r="EX8"/>
+      <c r="EY8"/>
+      <c r="EZ8"/>
+      <c r="FA8"/>
+      <c r="FB8"/>
+      <c r="FC8"/>
+      <c r="FD8"/>
+      <c r="FE8"/>
+      <c r="FF8"/>
+      <c r="FG8"/>
+      <c r="FH8"/>
+      <c r="FI8"/>
+      <c r="FJ8"/>
+      <c r="FK8"/>
+      <c r="FL8"/>
+      <c r="FM8"/>
+      <c r="FN8"/>
+      <c r="FO8"/>
+      <c r="FP8"/>
+      <c r="FQ8"/>
+      <c r="FR8"/>
+      <c r="FS8"/>
+      <c r="FT8"/>
+      <c r="FU8"/>
+      <c r="FV8"/>
+      <c r="FW8"/>
+      <c r="FX8"/>
+      <c r="FY8"/>
+      <c r="FZ8"/>
+      <c r="GA8"/>
+      <c r="GB8"/>
+      <c r="GC8"/>
+      <c r="GD8"/>
+      <c r="GE8"/>
+      <c r="GF8"/>
+      <c r="GG8"/>
+      <c r="GH8"/>
+      <c r="GI8"/>
+      <c r="GJ8"/>
+      <c r="GK8"/>
+      <c r="GL8"/>
+      <c r="GM8"/>
+      <c r="GN8"/>
+      <c r="GO8"/>
+      <c r="GP8"/>
+      <c r="GQ8"/>
+      <c r="GR8"/>
+      <c r="GS8"/>
+      <c r="GT8"/>
+      <c r="GU8"/>
+      <c r="GV8"/>
+      <c r="GW8"/>
+      <c r="GX8"/>
+      <c r="GY8"/>
+      <c r="GZ8"/>
+      <c r="HA8"/>
+      <c r="HB8"/>
+      <c r="HC8"/>
+      <c r="HD8"/>
+      <c r="HE8"/>
+      <c r="HF8"/>
+      <c r="HG8"/>
+      <c r="HH8"/>
+      <c r="HI8"/>
+      <c r="HJ8"/>
+      <c r="HK8"/>
+      <c r="HL8"/>
+      <c r="HM8"/>
+      <c r="HN8"/>
+      <c r="HO8"/>
+      <c r="HP8"/>
+      <c r="HQ8"/>
+      <c r="HR8"/>
+      <c r="HS8"/>
+      <c r="HT8"/>
+      <c r="HU8"/>
+      <c r="HV8"/>
+      <c r="HW8"/>
+      <c r="HX8"/>
+      <c r="HY8"/>
+      <c r="HZ8"/>
+      <c r="IA8"/>
+      <c r="IB8"/>
+      <c r="IC8"/>
+      <c r="ID8"/>
+      <c r="IE8"/>
+      <c r="IF8"/>
+      <c r="IG8"/>
+      <c r="IH8"/>
+      <c r="II8"/>
+      <c r="IJ8"/>
+      <c r="IK8"/>
+      <c r="IL8"/>
+      <c r="IM8"/>
+      <c r="IN8"/>
+      <c r="IO8"/>
+      <c r="IP8"/>
+      <c r="IQ8"/>
+      <c r="IR8"/>
+      <c r="IS8"/>
+      <c r="IT8"/>
+      <c r="IU8"/>
+      <c r="IV8"/>
     </row>
     <row r="9" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>50</v>
-      </c>
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
-      <c r="G9" s="23" t="s">
-        <v>45</v>
-      </c>
+      <c r="G9" s="23"/>
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
-      <c r="L9" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="L9" s="23"/>
       <c r="M9" s="23"/>
       <c r="N9" s="23"/>
       <c r="O9" s="23"/>
@@ -4161,16 +4401,16 @@
         <v>27</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
       <c r="G10" s="23" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
@@ -4197,18 +4437,28 @@
       <c r="AB10" s="25"/>
     </row>
     <row r="11" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
+      <c r="A11" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>51</v>
+      </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
+      <c r="G11" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
       <c r="J11" s="23"/>
       <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
+      <c r="L11" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
@@ -4227,124 +4477,114 @@
       <c r="AB11" s="25"/>
     </row>
     <row r="12" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="26"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
+      <c r="AA12" s="23"/>
+      <c r="AB12" s="25"/>
     </row>
     <row r="13" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
+    </row>
+    <row r="14" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B14" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C14" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="29" t="s">
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="31"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="31"/>
-      <c r="Y13" s="31"/>
-      <c r="Z13" s="31"/>
-      <c r="AA13" s="31"/>
-      <c r="AB13" s="32"/>
-    </row>
-    <row r="14" spans="1:256" ht="59" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="33" t="s">
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="32"/>
+    </row>
+    <row r="15" spans="1:256" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B15" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C15" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="37"/>
-      <c r="X14" s="37"/>
-      <c r="Y14" s="37"/>
-      <c r="Z14" s="37"/>
-      <c r="AA14" s="37"/>
-      <c r="AB14" s="38"/>
-    </row>
-    <row r="15" spans="1:256" ht="59" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="84" t="s">
-        <v>177</v>
-      </c>
-      <c r="B15" s="85" t="s">
-        <v>178</v>
-      </c>
-      <c r="C15" s="86" t="s">
-        <v>179</v>
-      </c>
-      <c r="D15" s="87" t="s">
-        <v>26</v>
-      </c>
+      <c r="D15" s="36"/>
       <c r="E15" s="37"/>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
@@ -4352,7 +4592,9 @@
       <c r="I15" s="37"/>
       <c r="J15" s="37"/>
       <c r="K15" s="37"/>
-      <c r="L15" s="34"/>
+      <c r="L15" s="34" t="s">
+        <v>25</v>
+      </c>
       <c r="M15" s="37"/>
       <c r="N15" s="37"/>
       <c r="O15" s="37"/>
@@ -4370,67 +4612,67 @@
       <c r="AA15" s="37"/>
       <c r="AB15" s="38"/>
     </row>
-    <row r="16" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:256" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="84" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="85" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="86" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="87" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="37"/>
+      <c r="W16" s="37"/>
+      <c r="X16" s="37"/>
+      <c r="Y16" s="37"/>
+      <c r="Z16" s="37"/>
+      <c r="AA16" s="37"/>
+      <c r="AB16" s="38"/>
+    </row>
+    <row r="17" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B17" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C17" s="30" t="s">
         <v>57</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="31"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="31"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="31"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="31"/>
-      <c r="Y16" s="31"/>
-      <c r="Z16" s="31"/>
-      <c r="AA16" s="31"/>
-      <c r="AB16" s="32"/>
-    </row>
-    <row r="17" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>61</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
+      <c r="F17" s="29"/>
       <c r="G17" s="31"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="31"/>
+      <c r="H17" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31" t="s">
+        <v>87</v>
+      </c>
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
       <c r="M17" s="31"/>
@@ -4452,13 +4694,13 @@
     </row>
     <row r="18" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="28" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>26</v>
@@ -4466,13 +4708,9 @@
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="31"/>
-      <c r="H18" s="29" t="s">
-        <v>58</v>
-      </c>
+      <c r="H18" s="29"/>
       <c r="I18" s="29"/>
-      <c r="J18" s="31" t="s">
-        <v>88</v>
-      </c>
+      <c r="J18" s="31"/>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
       <c r="M18" s="31"/>
@@ -4494,25 +4732,29 @@
     </row>
     <row r="19" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="28" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="29" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="29"/>
+      <c r="J19" s="31" t="s">
+        <v>88</v>
+      </c>
       <c r="K19" s="31"/>
-      <c r="L19" s="29"/>
+      <c r="L19" s="31"/>
       <c r="M19" s="31"/>
       <c r="N19" s="31"/>
       <c r="O19" s="31"/>
@@ -4534,23 +4776,23 @@
       <c r="A20" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="28" t="s">
-        <v>64</v>
+      <c r="B20" s="29" t="s">
+        <v>63</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="31" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
+      <c r="G20" s="29"/>
       <c r="H20" s="31"/>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
+      <c r="L20" s="29"/>
       <c r="M20" s="31"/>
       <c r="N20" s="31"/>
       <c r="O20" s="31"/>
@@ -4570,11 +4812,17 @@
     </row>
     <row r="21" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="28" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="31"/>
+      <c r="B21" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
@@ -4600,325 +4848,315 @@
       <c r="AA21" s="31"/>
       <c r="AB21" s="32"/>
     </row>
-    <row r="22" spans="1:256" s="81" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="76"/>
-      <c r="B22" s="77"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="77"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="77"/>
-      <c r="L22" s="77"/>
-      <c r="M22" s="77"/>
-      <c r="N22" s="77"/>
-      <c r="O22" s="77"/>
-      <c r="P22" s="77"/>
-      <c r="Q22" s="77"/>
-      <c r="R22" s="77"/>
-      <c r="S22" s="77"/>
-      <c r="T22" s="77"/>
-      <c r="U22" s="77"/>
-      <c r="V22" s="77"/>
-      <c r="W22" s="77"/>
-      <c r="X22" s="77"/>
-      <c r="Y22" s="77"/>
-      <c r="Z22" s="77"/>
-      <c r="AA22" s="77"/>
-      <c r="AB22" s="79"/>
-      <c r="AC22" s="80"/>
-      <c r="AD22" s="80"/>
-      <c r="AE22" s="80"/>
-      <c r="AF22" s="80"/>
-      <c r="AG22" s="80"/>
-      <c r="AH22" s="80"/>
-      <c r="AI22" s="80"/>
-      <c r="AJ22" s="80"/>
-      <c r="AK22" s="80"/>
-      <c r="AL22" s="80"/>
-      <c r="AM22" s="80"/>
-      <c r="AN22" s="80"/>
-      <c r="AO22" s="80"/>
-      <c r="AP22" s="80"/>
-      <c r="AQ22" s="80"/>
-      <c r="AR22" s="80"/>
-      <c r="AS22" s="80"/>
-      <c r="AT22" s="80"/>
-      <c r="AU22" s="80"/>
-      <c r="AV22" s="80"/>
-      <c r="AW22" s="80"/>
-      <c r="AX22" s="80"/>
-      <c r="AY22" s="80"/>
-      <c r="AZ22" s="80"/>
-      <c r="BA22" s="80"/>
-      <c r="BB22" s="80"/>
-      <c r="BC22" s="80"/>
-      <c r="BD22" s="80"/>
-      <c r="BE22" s="80"/>
-      <c r="BF22" s="80"/>
-      <c r="BG22" s="80"/>
-      <c r="BH22" s="80"/>
-      <c r="BI22" s="80"/>
-      <c r="BJ22" s="80"/>
-      <c r="BK22" s="80"/>
-      <c r="BL22" s="80"/>
-      <c r="BM22" s="80"/>
-      <c r="BN22" s="80"/>
-      <c r="BO22" s="80"/>
-      <c r="BP22" s="80"/>
-      <c r="BQ22" s="80"/>
-      <c r="BR22" s="80"/>
-      <c r="BS22" s="80"/>
-      <c r="BT22" s="80"/>
-      <c r="BU22" s="80"/>
-      <c r="BV22" s="80"/>
-      <c r="BW22" s="80"/>
-      <c r="BX22" s="80"/>
-      <c r="BY22" s="80"/>
-      <c r="BZ22" s="80"/>
-      <c r="CA22" s="80"/>
-      <c r="CB22" s="80"/>
-      <c r="CC22" s="80"/>
-      <c r="CD22" s="80"/>
-      <c r="CE22" s="80"/>
-      <c r="CF22" s="80"/>
-      <c r="CG22" s="80"/>
-      <c r="CH22" s="80"/>
-      <c r="CI22" s="80"/>
-      <c r="CJ22" s="80"/>
-      <c r="CK22" s="80"/>
-      <c r="CL22" s="80"/>
-      <c r="CM22" s="80"/>
-      <c r="CN22" s="80"/>
-      <c r="CO22" s="80"/>
-      <c r="CP22" s="80"/>
-      <c r="CQ22" s="80"/>
-      <c r="CR22" s="80"/>
-      <c r="CS22" s="80"/>
-      <c r="CT22" s="80"/>
-      <c r="CU22" s="80"/>
-      <c r="CV22" s="80"/>
-      <c r="CW22" s="80"/>
-      <c r="CX22" s="80"/>
-      <c r="CY22" s="80"/>
-      <c r="CZ22" s="80"/>
-      <c r="DA22" s="80"/>
-      <c r="DB22" s="80"/>
-      <c r="DC22" s="80"/>
-      <c r="DD22" s="80"/>
-      <c r="DE22" s="80"/>
-      <c r="DF22" s="80"/>
-      <c r="DG22" s="80"/>
-      <c r="DH22" s="80"/>
-      <c r="DI22" s="80"/>
-      <c r="DJ22" s="80"/>
-      <c r="DK22" s="80"/>
-      <c r="DL22" s="80"/>
-      <c r="DM22" s="80"/>
-      <c r="DN22" s="80"/>
-      <c r="DO22" s="80"/>
-      <c r="DP22" s="80"/>
-      <c r="DQ22" s="80"/>
-      <c r="DR22" s="80"/>
-      <c r="DS22" s="80"/>
-      <c r="DT22" s="80"/>
-      <c r="DU22" s="80"/>
-      <c r="DV22" s="80"/>
-      <c r="DW22" s="80"/>
-      <c r="DX22" s="80"/>
-      <c r="DY22" s="80"/>
-      <c r="DZ22" s="80"/>
-      <c r="EA22" s="80"/>
-      <c r="EB22" s="80"/>
-      <c r="EC22" s="80"/>
-      <c r="ED22" s="80"/>
-      <c r="EE22" s="80"/>
-      <c r="EF22" s="80"/>
-      <c r="EG22" s="80"/>
-      <c r="EH22" s="80"/>
-      <c r="EI22" s="80"/>
-      <c r="EJ22" s="80"/>
-      <c r="EK22" s="80"/>
-      <c r="EL22" s="80"/>
-      <c r="EM22" s="80"/>
-      <c r="EN22" s="80"/>
-      <c r="EO22" s="80"/>
-      <c r="EP22" s="80"/>
-      <c r="EQ22" s="80"/>
-      <c r="ER22" s="80"/>
-      <c r="ES22" s="80"/>
-      <c r="ET22" s="80"/>
-      <c r="EU22" s="80"/>
-      <c r="EV22" s="80"/>
-      <c r="EW22" s="80"/>
-      <c r="EX22" s="80"/>
-      <c r="EY22" s="80"/>
-      <c r="EZ22" s="80"/>
-      <c r="FA22" s="80"/>
-      <c r="FB22" s="80"/>
-      <c r="FC22" s="80"/>
-      <c r="FD22" s="80"/>
-      <c r="FE22" s="80"/>
-      <c r="FF22" s="80"/>
-      <c r="FG22" s="80"/>
-      <c r="FH22" s="80"/>
-      <c r="FI22" s="80"/>
-      <c r="FJ22" s="80"/>
-      <c r="FK22" s="80"/>
-      <c r="FL22" s="80"/>
-      <c r="FM22" s="80"/>
-      <c r="FN22" s="80"/>
-      <c r="FO22" s="80"/>
-      <c r="FP22" s="80"/>
-      <c r="FQ22" s="80"/>
-      <c r="FR22" s="80"/>
-      <c r="FS22" s="80"/>
-      <c r="FT22" s="80"/>
-      <c r="FU22" s="80"/>
-      <c r="FV22" s="80"/>
-      <c r="FW22" s="80"/>
-      <c r="FX22" s="80"/>
-      <c r="FY22" s="80"/>
-      <c r="FZ22" s="80"/>
-      <c r="GA22" s="80"/>
-      <c r="GB22" s="80"/>
-      <c r="GC22" s="80"/>
-      <c r="GD22" s="80"/>
-      <c r="GE22" s="80"/>
-      <c r="GF22" s="80"/>
-      <c r="GG22" s="80"/>
-      <c r="GH22" s="80"/>
-      <c r="GI22" s="80"/>
-      <c r="GJ22" s="80"/>
-      <c r="GK22" s="80"/>
-      <c r="GL22" s="80"/>
-      <c r="GM22" s="80"/>
-      <c r="GN22" s="80"/>
-      <c r="GO22" s="80"/>
-      <c r="GP22" s="80"/>
-      <c r="GQ22" s="80"/>
-      <c r="GR22" s="80"/>
-      <c r="GS22" s="80"/>
-      <c r="GT22" s="80"/>
-      <c r="GU22" s="80"/>
-      <c r="GV22" s="80"/>
-      <c r="GW22" s="80"/>
-      <c r="GX22" s="80"/>
-      <c r="GY22" s="80"/>
-      <c r="GZ22" s="80"/>
-      <c r="HA22" s="80"/>
-      <c r="HB22" s="80"/>
-      <c r="HC22" s="80"/>
-      <c r="HD22" s="80"/>
-      <c r="HE22" s="80"/>
-      <c r="HF22" s="80"/>
-      <c r="HG22" s="80"/>
-      <c r="HH22" s="80"/>
-      <c r="HI22" s="80"/>
-      <c r="HJ22" s="80"/>
-      <c r="HK22" s="80"/>
-      <c r="HL22" s="80"/>
-      <c r="HM22" s="80"/>
-      <c r="HN22" s="80"/>
-      <c r="HO22" s="80"/>
-      <c r="HP22" s="80"/>
-      <c r="HQ22" s="80"/>
-      <c r="HR22" s="80"/>
-      <c r="HS22" s="80"/>
-      <c r="HT22" s="80"/>
-      <c r="HU22" s="80"/>
-      <c r="HV22" s="80"/>
-      <c r="HW22" s="80"/>
-      <c r="HX22" s="80"/>
-      <c r="HY22" s="80"/>
-      <c r="HZ22" s="80"/>
-      <c r="IA22" s="80"/>
-      <c r="IB22" s="80"/>
-      <c r="IC22" s="80"/>
-      <c r="ID22" s="80"/>
-      <c r="IE22" s="80"/>
-      <c r="IF22" s="80"/>
-      <c r="IG22" s="80"/>
-      <c r="IH22" s="80"/>
-      <c r="II22" s="80"/>
-      <c r="IJ22" s="80"/>
-      <c r="IK22" s="80"/>
-      <c r="IL22" s="80"/>
-      <c r="IM22" s="80"/>
-      <c r="IN22" s="80"/>
-      <c r="IO22" s="80"/>
-      <c r="IP22" s="80"/>
-      <c r="IQ22" s="80"/>
-      <c r="IR22" s="80"/>
-      <c r="IS22" s="80"/>
-      <c r="IT22" s="80"/>
-      <c r="IU22" s="80"/>
-      <c r="IV22" s="80"/>
-    </row>
-    <row r="23" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="33" t="s">
+    <row r="22" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="31"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="32"/>
+    </row>
+    <row r="23" spans="1:256" s="81" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="76"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="77"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77"/>
+      <c r="N23" s="77"/>
+      <c r="O23" s="77"/>
+      <c r="P23" s="77"/>
+      <c r="Q23" s="77"/>
+      <c r="R23" s="77"/>
+      <c r="S23" s="77"/>
+      <c r="T23" s="77"/>
+      <c r="U23" s="77"/>
+      <c r="V23" s="77"/>
+      <c r="W23" s="77"/>
+      <c r="X23" s="77"/>
+      <c r="Y23" s="77"/>
+      <c r="Z23" s="77"/>
+      <c r="AA23" s="77"/>
+      <c r="AB23" s="79"/>
+      <c r="AC23" s="80"/>
+      <c r="AD23" s="80"/>
+      <c r="AE23" s="80"/>
+      <c r="AF23" s="80"/>
+      <c r="AG23" s="80"/>
+      <c r="AH23" s="80"/>
+      <c r="AI23" s="80"/>
+      <c r="AJ23" s="80"/>
+      <c r="AK23" s="80"/>
+      <c r="AL23" s="80"/>
+      <c r="AM23" s="80"/>
+      <c r="AN23" s="80"/>
+      <c r="AO23" s="80"/>
+      <c r="AP23" s="80"/>
+      <c r="AQ23" s="80"/>
+      <c r="AR23" s="80"/>
+      <c r="AS23" s="80"/>
+      <c r="AT23" s="80"/>
+      <c r="AU23" s="80"/>
+      <c r="AV23" s="80"/>
+      <c r="AW23" s="80"/>
+      <c r="AX23" s="80"/>
+      <c r="AY23" s="80"/>
+      <c r="AZ23" s="80"/>
+      <c r="BA23" s="80"/>
+      <c r="BB23" s="80"/>
+      <c r="BC23" s="80"/>
+      <c r="BD23" s="80"/>
+      <c r="BE23" s="80"/>
+      <c r="BF23" s="80"/>
+      <c r="BG23" s="80"/>
+      <c r="BH23" s="80"/>
+      <c r="BI23" s="80"/>
+      <c r="BJ23" s="80"/>
+      <c r="BK23" s="80"/>
+      <c r="BL23" s="80"/>
+      <c r="BM23" s="80"/>
+      <c r="BN23" s="80"/>
+      <c r="BO23" s="80"/>
+      <c r="BP23" s="80"/>
+      <c r="BQ23" s="80"/>
+      <c r="BR23" s="80"/>
+      <c r="BS23" s="80"/>
+      <c r="BT23" s="80"/>
+      <c r="BU23" s="80"/>
+      <c r="BV23" s="80"/>
+      <c r="BW23" s="80"/>
+      <c r="BX23" s="80"/>
+      <c r="BY23" s="80"/>
+      <c r="BZ23" s="80"/>
+      <c r="CA23" s="80"/>
+      <c r="CB23" s="80"/>
+      <c r="CC23" s="80"/>
+      <c r="CD23" s="80"/>
+      <c r="CE23" s="80"/>
+      <c r="CF23" s="80"/>
+      <c r="CG23" s="80"/>
+      <c r="CH23" s="80"/>
+      <c r="CI23" s="80"/>
+      <c r="CJ23" s="80"/>
+      <c r="CK23" s="80"/>
+      <c r="CL23" s="80"/>
+      <c r="CM23" s="80"/>
+      <c r="CN23" s="80"/>
+      <c r="CO23" s="80"/>
+      <c r="CP23" s="80"/>
+      <c r="CQ23" s="80"/>
+      <c r="CR23" s="80"/>
+      <c r="CS23" s="80"/>
+      <c r="CT23" s="80"/>
+      <c r="CU23" s="80"/>
+      <c r="CV23" s="80"/>
+      <c r="CW23" s="80"/>
+      <c r="CX23" s="80"/>
+      <c r="CY23" s="80"/>
+      <c r="CZ23" s="80"/>
+      <c r="DA23" s="80"/>
+      <c r="DB23" s="80"/>
+      <c r="DC23" s="80"/>
+      <c r="DD23" s="80"/>
+      <c r="DE23" s="80"/>
+      <c r="DF23" s="80"/>
+      <c r="DG23" s="80"/>
+      <c r="DH23" s="80"/>
+      <c r="DI23" s="80"/>
+      <c r="DJ23" s="80"/>
+      <c r="DK23" s="80"/>
+      <c r="DL23" s="80"/>
+      <c r="DM23" s="80"/>
+      <c r="DN23" s="80"/>
+      <c r="DO23" s="80"/>
+      <c r="DP23" s="80"/>
+      <c r="DQ23" s="80"/>
+      <c r="DR23" s="80"/>
+      <c r="DS23" s="80"/>
+      <c r="DT23" s="80"/>
+      <c r="DU23" s="80"/>
+      <c r="DV23" s="80"/>
+      <c r="DW23" s="80"/>
+      <c r="DX23" s="80"/>
+      <c r="DY23" s="80"/>
+      <c r="DZ23" s="80"/>
+      <c r="EA23" s="80"/>
+      <c r="EB23" s="80"/>
+      <c r="EC23" s="80"/>
+      <c r="ED23" s="80"/>
+      <c r="EE23" s="80"/>
+      <c r="EF23" s="80"/>
+      <c r="EG23" s="80"/>
+      <c r="EH23" s="80"/>
+      <c r="EI23" s="80"/>
+      <c r="EJ23" s="80"/>
+      <c r="EK23" s="80"/>
+      <c r="EL23" s="80"/>
+      <c r="EM23" s="80"/>
+      <c r="EN23" s="80"/>
+      <c r="EO23" s="80"/>
+      <c r="EP23" s="80"/>
+      <c r="EQ23" s="80"/>
+      <c r="ER23" s="80"/>
+      <c r="ES23" s="80"/>
+      <c r="ET23" s="80"/>
+      <c r="EU23" s="80"/>
+      <c r="EV23" s="80"/>
+      <c r="EW23" s="80"/>
+      <c r="EX23" s="80"/>
+      <c r="EY23" s="80"/>
+      <c r="EZ23" s="80"/>
+      <c r="FA23" s="80"/>
+      <c r="FB23" s="80"/>
+      <c r="FC23" s="80"/>
+      <c r="FD23" s="80"/>
+      <c r="FE23" s="80"/>
+      <c r="FF23" s="80"/>
+      <c r="FG23" s="80"/>
+      <c r="FH23" s="80"/>
+      <c r="FI23" s="80"/>
+      <c r="FJ23" s="80"/>
+      <c r="FK23" s="80"/>
+      <c r="FL23" s="80"/>
+      <c r="FM23" s="80"/>
+      <c r="FN23" s="80"/>
+      <c r="FO23" s="80"/>
+      <c r="FP23" s="80"/>
+      <c r="FQ23" s="80"/>
+      <c r="FR23" s="80"/>
+      <c r="FS23" s="80"/>
+      <c r="FT23" s="80"/>
+      <c r="FU23" s="80"/>
+      <c r="FV23" s="80"/>
+      <c r="FW23" s="80"/>
+      <c r="FX23" s="80"/>
+      <c r="FY23" s="80"/>
+      <c r="FZ23" s="80"/>
+      <c r="GA23" s="80"/>
+      <c r="GB23" s="80"/>
+      <c r="GC23" s="80"/>
+      <c r="GD23" s="80"/>
+      <c r="GE23" s="80"/>
+      <c r="GF23" s="80"/>
+      <c r="GG23" s="80"/>
+      <c r="GH23" s="80"/>
+      <c r="GI23" s="80"/>
+      <c r="GJ23" s="80"/>
+      <c r="GK23" s="80"/>
+      <c r="GL23" s="80"/>
+      <c r="GM23" s="80"/>
+      <c r="GN23" s="80"/>
+      <c r="GO23" s="80"/>
+      <c r="GP23" s="80"/>
+      <c r="GQ23" s="80"/>
+      <c r="GR23" s="80"/>
+      <c r="GS23" s="80"/>
+      <c r="GT23" s="80"/>
+      <c r="GU23" s="80"/>
+      <c r="GV23" s="80"/>
+      <c r="GW23" s="80"/>
+      <c r="GX23" s="80"/>
+      <c r="GY23" s="80"/>
+      <c r="GZ23" s="80"/>
+      <c r="HA23" s="80"/>
+      <c r="HB23" s="80"/>
+      <c r="HC23" s="80"/>
+      <c r="HD23" s="80"/>
+      <c r="HE23" s="80"/>
+      <c r="HF23" s="80"/>
+      <c r="HG23" s="80"/>
+      <c r="HH23" s="80"/>
+      <c r="HI23" s="80"/>
+      <c r="HJ23" s="80"/>
+      <c r="HK23" s="80"/>
+      <c r="HL23" s="80"/>
+      <c r="HM23" s="80"/>
+      <c r="HN23" s="80"/>
+      <c r="HO23" s="80"/>
+      <c r="HP23" s="80"/>
+      <c r="HQ23" s="80"/>
+      <c r="HR23" s="80"/>
+      <c r="HS23" s="80"/>
+      <c r="HT23" s="80"/>
+      <c r="HU23" s="80"/>
+      <c r="HV23" s="80"/>
+      <c r="HW23" s="80"/>
+      <c r="HX23" s="80"/>
+      <c r="HY23" s="80"/>
+      <c r="HZ23" s="80"/>
+      <c r="IA23" s="80"/>
+      <c r="IB23" s="80"/>
+      <c r="IC23" s="80"/>
+      <c r="ID23" s="80"/>
+      <c r="IE23" s="80"/>
+      <c r="IF23" s="80"/>
+      <c r="IG23" s="80"/>
+      <c r="IH23" s="80"/>
+      <c r="II23" s="80"/>
+      <c r="IJ23" s="80"/>
+      <c r="IK23" s="80"/>
+      <c r="IL23" s="80"/>
+      <c r="IM23" s="80"/>
+      <c r="IN23" s="80"/>
+      <c r="IO23" s="80"/>
+      <c r="IP23" s="80"/>
+      <c r="IQ23" s="80"/>
+      <c r="IR23" s="80"/>
+      <c r="IS23" s="80"/>
+      <c r="IT23" s="80"/>
+      <c r="IU23" s="80"/>
+      <c r="IV23" s="80"/>
+    </row>
+    <row r="24" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B24" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C24" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29" t="s">
+      <c r="D24" s="37"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="31"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31"/>
-      <c r="X23" s="31"/>
-      <c r="Y23" s="31"/>
-      <c r="Z23" s="31"/>
-      <c r="AA23" s="31"/>
-      <c r="AB23" s="32"/>
-    </row>
-    <row r="24" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
       <c r="G24" s="31"/>
-      <c r="H24" s="31" t="s">
-        <v>85</v>
-      </c>
+      <c r="H24" s="31"/>
       <c r="I24" s="31"/>
-      <c r="J24" s="34" t="s">
-        <v>86</v>
-      </c>
+      <c r="J24" s="31"/>
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="31"/>
@@ -4940,13 +5178,13 @@
     </row>
     <row r="25" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="33" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D25" s="37" t="s">
         <v>26</v>
@@ -4955,11 +5193,11 @@
       <c r="F25" s="29"/>
       <c r="G25" s="31"/>
       <c r="H25" s="31" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="I25" s="31"/>
       <c r="J25" s="34" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
@@ -4985,10 +5223,10 @@
         <v>55</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D26" s="37" t="s">
         <v>26</v>
@@ -5027,10 +5265,10 @@
         <v>55</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D27" s="37" t="s">
         <v>26</v>
@@ -5038,10 +5276,12 @@
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
+      <c r="H27" s="31" t="s">
+        <v>58</v>
+      </c>
       <c r="I27" s="31"/>
       <c r="J27" s="34" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
@@ -5067,10 +5307,10 @@
         <v>55</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D28" s="37" t="s">
         <v>26</v>
@@ -5107,10 +5347,10 @@
         <v>55</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D29" s="37" t="s">
         <v>26</v>
@@ -5147,10 +5387,10 @@
         <v>55</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>26</v>
@@ -5187,10 +5427,10 @@
         <v>55</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D31" s="37" t="s">
         <v>26</v>
@@ -5198,12 +5438,10 @@
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
       <c r="G31" s="31"/>
-      <c r="H31" s="31" t="s">
-        <v>58</v>
-      </c>
+      <c r="H31" s="31"/>
       <c r="I31" s="31"/>
       <c r="J31" s="34" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="K31" s="31"/>
       <c r="L31" s="31"/>
@@ -5229,10 +5467,10 @@
         <v>55</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C32" s="35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D32" s="37" t="s">
         <v>26</v>
@@ -5240,10 +5478,12 @@
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
       <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
+      <c r="H32" s="31" t="s">
+        <v>58</v>
+      </c>
       <c r="I32" s="31"/>
       <c r="J32" s="34" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="K32" s="31"/>
       <c r="L32" s="31"/>
@@ -5269,10 +5509,10 @@
         <v>55</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D33" s="37" t="s">
         <v>26</v>
@@ -5309,10 +5549,10 @@
         <v>55</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D34" s="37" t="s">
         <v>26</v>
@@ -5349,10 +5589,10 @@
         <v>55</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D35" s="37" t="s">
         <v>26</v>
@@ -5389,10 +5629,10 @@
         <v>55</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D36" s="37" t="s">
         <v>26</v>
@@ -5429,10 +5669,10 @@
         <v>55</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D37" s="37" t="s">
         <v>26</v>
@@ -5469,10 +5709,10 @@
         <v>55</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>115</v>
+        <v>159</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D38" s="37" t="s">
         <v>26</v>
@@ -5483,7 +5723,7 @@
       <c r="H38" s="31"/>
       <c r="I38" s="31"/>
       <c r="J38" s="34" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="K38" s="31"/>
       <c r="L38" s="31"/>
@@ -5506,17 +5746,25 @@
     </row>
     <row r="39" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="33" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
+      <c r="B39" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
       <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
+      <c r="J39" s="34" t="s">
+        <v>117</v>
+      </c>
       <c r="K39" s="31"/>
       <c r="L39" s="31"/>
       <c r="M39" s="31"/>
@@ -5537,7 +5785,9 @@
       <c r="AB39" s="32"/>
     </row>
     <row r="40" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="40"/>
+      <c r="A40" s="33" t="s">
+        <v>28</v>
+      </c>
       <c r="B40" s="37"/>
       <c r="C40" s="36"/>
       <c r="D40" s="37"/>
@@ -5567,153 +5817,147 @@
       <c r="AB40" s="32"/>
     </row>
     <row r="41" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="26"/>
-      <c r="M41" s="26"/>
-      <c r="N41" s="26"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="26"/>
-      <c r="Q41" s="26"/>
-      <c r="R41" s="26"/>
-      <c r="S41" s="26"/>
-      <c r="T41" s="26"/>
-      <c r="U41" s="26"/>
-      <c r="V41" s="26"/>
-      <c r="W41" s="26"/>
-      <c r="X41" s="26"/>
-      <c r="Y41" s="26"/>
-      <c r="Z41" s="26"/>
-      <c r="AA41" s="26"/>
-      <c r="AB41" s="26"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="32"/>
     </row>
     <row r="42" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="26"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="26"/>
+      <c r="T42" s="26"/>
+      <c r="U42" s="26"/>
+      <c r="V42" s="26"/>
+      <c r="W42" s="26"/>
+      <c r="X42" s="26"/>
+      <c r="Y42" s="26"/>
+      <c r="Z42" s="26"/>
+      <c r="AA42" s="26"/>
+      <c r="AB42" s="26"/>
+    </row>
+    <row r="43" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B43" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C43" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="42" t="s">
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="42" t="s">
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44"/>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="44"/>
-      <c r="S42" s="44"/>
-      <c r="T42" s="44"/>
-      <c r="U42" s="44"/>
-      <c r="V42" s="44"/>
-      <c r="W42" s="44"/>
-      <c r="X42" s="44"/>
-      <c r="Y42" s="44"/>
-      <c r="Z42" s="44"/>
-      <c r="AA42" s="44"/>
-      <c r="AB42" s="45"/>
-    </row>
-    <row r="43" spans="1:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="46" t="s">
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+      <c r="T43" s="44"/>
+      <c r="U43" s="44"/>
+      <c r="V43" s="44"/>
+      <c r="W43" s="44"/>
+      <c r="X43" s="44"/>
+      <c r="Y43" s="44"/>
+      <c r="Z43" s="44"/>
+      <c r="AA43" s="44"/>
+      <c r="AB43" s="45"/>
+    </row>
+    <row r="44" spans="1:28" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B44" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="63" t="s">
+      <c r="C44" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
-      <c r="R43" s="48"/>
-      <c r="S43" s="48"/>
-      <c r="T43" s="48"/>
-      <c r="U43" s="48"/>
-      <c r="V43" s="48"/>
-      <c r="W43" s="48"/>
-      <c r="X43" s="48"/>
-      <c r="Y43" s="48"/>
-      <c r="Z43" s="48"/>
-      <c r="AA43" s="48"/>
-      <c r="AB43" s="49"/>
-    </row>
-    <row r="44" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="50"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="44"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
-      <c r="O44" s="44"/>
-      <c r="P44" s="44"/>
-      <c r="Q44" s="44"/>
-      <c r="R44" s="44"/>
-      <c r="S44" s="44"/>
-      <c r="T44" s="44"/>
-      <c r="U44" s="44"/>
-      <c r="V44" s="44"/>
-      <c r="W44" s="44"/>
-      <c r="X44" s="44"/>
-      <c r="Y44" s="44"/>
-      <c r="Z44" s="44"/>
-      <c r="AA44" s="44"/>
-      <c r="AB44" s="45"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="48"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="48"/>
+      <c r="O44" s="48"/>
+      <c r="P44" s="48"/>
+      <c r="Q44" s="48"/>
+      <c r="R44" s="48"/>
+      <c r="S44" s="48"/>
+      <c r="T44" s="48"/>
+      <c r="U44" s="48"/>
+      <c r="V44" s="48"/>
+      <c r="W44" s="48"/>
+      <c r="X44" s="48"/>
+      <c r="Y44" s="48"/>
+      <c r="Z44" s="48"/>
+      <c r="AA44" s="48"/>
+      <c r="AB44" s="49"/>
     </row>
     <row r="45" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45" s="51" t="s">
-        <v>122</v>
-      </c>
+      <c r="A45" s="50"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="51"/>
       <c r="D45" s="44"/>
-      <c r="E45" s="42"/>
+      <c r="E45" s="44"/>
       <c r="F45" s="44"/>
       <c r="G45" s="44"/>
       <c r="H45" s="44"/>
@@ -5740,16 +5984,16 @@
     </row>
     <row r="46" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
-      <c r="C46" s="43" t="s">
-        <v>131</v>
+      <c r="C46" s="51" t="s">
+        <v>122</v>
       </c>
       <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
+      <c r="E46" s="42"/>
       <c r="F46" s="44"/>
       <c r="G46" s="44"/>
       <c r="H46" s="44"/>
@@ -5779,10 +6023,10 @@
         <v>23</v>
       </c>
       <c r="B47" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C47" s="43" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D47" s="44"/>
       <c r="E47" s="44"/>
@@ -5815,10 +6059,10 @@
         <v>23</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C48" s="43" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D48" s="44"/>
       <c r="E48" s="44"/>
@@ -5851,10 +6095,10 @@
         <v>23</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C49" s="43" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D49" s="44"/>
       <c r="E49" s="44"/>
@@ -5887,10 +6131,10 @@
         <v>23</v>
       </c>
       <c r="B50" s="42" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C50" s="43" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D50" s="44"/>
       <c r="E50" s="44"/>
@@ -5920,10 +6164,14 @@
     </row>
     <row r="51" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="41" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
-      <c r="B51" s="44"/>
-      <c r="C51" s="51"/>
+      <c r="B51" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="43" t="s">
+        <v>130</v>
+      </c>
       <c r="D51" s="44"/>
       <c r="E51" s="44"/>
       <c r="F51" s="44"/>
@@ -5951,7 +6199,9 @@
       <c r="AB51" s="45"/>
     </row>
     <row r="52" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="50"/>
+      <c r="A52" s="41" t="s">
+        <v>28</v>
+      </c>
       <c r="B52" s="44"/>
       <c r="C52" s="51"/>
       <c r="D52" s="44"/>
@@ -5981,17 +6231,11 @@
       <c r="AB52" s="45"/>
     </row>
     <row r="53" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B53" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" s="51" t="s">
-        <v>82</v>
-      </c>
+      <c r="A53" s="50"/>
+      <c r="B53" s="44"/>
+      <c r="C53" s="51"/>
       <c r="D53" s="44"/>
-      <c r="E53" s="42"/>
+      <c r="E53" s="44"/>
       <c r="F53" s="44"/>
       <c r="G53" s="44"/>
       <c r="H53" s="44"/>
@@ -6018,16 +6262,16 @@
     </row>
     <row r="54" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
-      <c r="C54" s="43" t="s">
-        <v>134</v>
+      <c r="C54" s="51" t="s">
+        <v>82</v>
       </c>
       <c r="D54" s="44"/>
-      <c r="E54" s="44"/>
+      <c r="E54" s="42"/>
       <c r="F54" s="44"/>
       <c r="G54" s="44"/>
       <c r="H54" s="44"/>
@@ -6057,10 +6301,10 @@
         <v>23</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C55" s="43" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="D55" s="44"/>
       <c r="E55" s="44"/>
@@ -6093,10 +6337,10 @@
         <v>23</v>
       </c>
       <c r="B56" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C56" s="43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D56" s="44"/>
       <c r="E56" s="44"/>
@@ -6129,10 +6373,10 @@
         <v>23</v>
       </c>
       <c r="B57" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C57" s="43" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="D57" s="44"/>
       <c r="E57" s="44"/>
@@ -6165,10 +6409,10 @@
         <v>23</v>
       </c>
       <c r="B58" s="42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C58" s="43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D58" s="44"/>
       <c r="E58" s="44"/>
@@ -6201,10 +6445,10 @@
         <v>23</v>
       </c>
       <c r="B59" s="42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D59" s="44"/>
       <c r="E59" s="44"/>
@@ -6237,10 +6481,10 @@
         <v>23</v>
       </c>
       <c r="B60" s="42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="D60" s="44"/>
       <c r="E60" s="44"/>
@@ -6273,10 +6517,10 @@
         <v>23</v>
       </c>
       <c r="B61" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="D61" s="44"/>
       <c r="E61" s="44"/>
@@ -6309,10 +6553,10 @@
         <v>23</v>
       </c>
       <c r="B62" s="42" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C62" s="43" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D62" s="44"/>
       <c r="E62" s="44"/>
@@ -6345,10 +6589,10 @@
         <v>23</v>
       </c>
       <c r="B63" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D63" s="44"/>
       <c r="E63" s="44"/>
@@ -6381,10 +6625,10 @@
         <v>23</v>
       </c>
       <c r="B64" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D64" s="44"/>
       <c r="E64" s="44"/>
@@ -6417,10 +6661,10 @@
         <v>23</v>
       </c>
       <c r="B65" s="42" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D65" s="44"/>
       <c r="E65" s="44"/>
@@ -6453,10 +6697,10 @@
         <v>23</v>
       </c>
       <c r="B66" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D66" s="44"/>
       <c r="E66" s="44"/>
@@ -6489,10 +6733,10 @@
         <v>23</v>
       </c>
       <c r="B67" s="42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D67" s="44"/>
       <c r="E67" s="44"/>
@@ -6525,10 +6769,10 @@
         <v>23</v>
       </c>
       <c r="B68" s="42" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D68" s="44"/>
       <c r="E68" s="44"/>
@@ -6558,10 +6802,14 @@
     </row>
     <row r="69" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="41" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
-      <c r="B69" s="44"/>
-      <c r="C69" s="51"/>
+      <c r="B69" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" s="43" t="s">
+        <v>163</v>
+      </c>
       <c r="D69" s="44"/>
       <c r="E69" s="44"/>
       <c r="F69" s="44"/>
@@ -6589,7 +6837,9 @@
       <c r="AB69" s="45"/>
     </row>
     <row r="70" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="50"/>
+      <c r="A70" s="41" t="s">
+        <v>28</v>
+      </c>
       <c r="B70" s="44"/>
       <c r="C70" s="51"/>
       <c r="D70" s="44"/>
@@ -6618,133 +6868,133 @@
       <c r="AA70" s="44"/>
       <c r="AB70" s="45"/>
     </row>
-    <row r="71" spans="1:28" ht="35.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="52" t="s">
+    <row r="71" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="50"/>
+      <c r="B71" s="44"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="44"/>
+      <c r="G71" s="44"/>
+      <c r="H71" s="44"/>
+      <c r="I71" s="44"/>
+      <c r="J71" s="44"/>
+      <c r="K71" s="44"/>
+      <c r="L71" s="44"/>
+      <c r="M71" s="44"/>
+      <c r="N71" s="44"/>
+      <c r="O71" s="44"/>
+      <c r="P71" s="44"/>
+      <c r="Q71" s="44"/>
+      <c r="R71" s="44"/>
+      <c r="S71" s="44"/>
+      <c r="T71" s="44"/>
+      <c r="U71" s="44"/>
+      <c r="V71" s="44"/>
+      <c r="W71" s="44"/>
+      <c r="X71" s="44"/>
+      <c r="Y71" s="44"/>
+      <c r="Z71" s="44"/>
+      <c r="AA71" s="44"/>
+      <c r="AB71" s="45"/>
+    </row>
+    <row r="72" spans="1:28" ht="35.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B71" s="53" t="s">
+      <c r="B72" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C71" s="47" t="s">
+      <c r="C72" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54"/>
-      <c r="F71" s="54"/>
-      <c r="G71" s="54"/>
-      <c r="H71" s="54"/>
-      <c r="I71" s="54"/>
-      <c r="J71" s="54"/>
-      <c r="K71" s="54"/>
-      <c r="L71" s="54"/>
-      <c r="M71" s="54"/>
-      <c r="N71" s="54"/>
-      <c r="O71" s="54"/>
-      <c r="P71" s="54"/>
-      <c r="Q71" s="54"/>
-      <c r="R71" s="54"/>
-      <c r="S71" s="54"/>
-      <c r="T71" s="54"/>
-      <c r="U71" s="54"/>
-      <c r="V71" s="54"/>
-      <c r="W71" s="54"/>
-      <c r="X71" s="54"/>
-      <c r="Y71" s="54"/>
-      <c r="Z71" s="54"/>
-      <c r="AA71" s="54"/>
-      <c r="AB71" s="55"/>
-    </row>
-    <row r="72" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="41" t="s">
+      <c r="D72" s="54"/>
+      <c r="E72" s="54"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+      <c r="I72" s="54"/>
+      <c r="J72" s="54"/>
+      <c r="K72" s="54"/>
+      <c r="L72" s="54"/>
+      <c r="M72" s="54"/>
+      <c r="N72" s="54"/>
+      <c r="O72" s="54"/>
+      <c r="P72" s="54"/>
+      <c r="Q72" s="54"/>
+      <c r="R72" s="54"/>
+      <c r="S72" s="54"/>
+      <c r="T72" s="54"/>
+      <c r="U72" s="54"/>
+      <c r="V72" s="54"/>
+      <c r="W72" s="54"/>
+      <c r="X72" s="54"/>
+      <c r="Y72" s="54"/>
+      <c r="Z72" s="54"/>
+      <c r="AA72" s="54"/>
+      <c r="AB72" s="55"/>
+    </row>
+    <row r="73" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B72" s="44"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="44"/>
-      <c r="G72" s="44"/>
-      <c r="H72" s="44"/>
-      <c r="I72" s="44"/>
-      <c r="J72" s="44"/>
-      <c r="K72" s="44"/>
-      <c r="L72" s="44"/>
-      <c r="M72" s="44"/>
-      <c r="N72" s="44"/>
-      <c r="O72" s="44"/>
-      <c r="P72" s="44"/>
-      <c r="Q72" s="44"/>
-      <c r="R72" s="44"/>
-      <c r="S72" s="44"/>
-      <c r="T72" s="44"/>
-      <c r="U72" s="44"/>
-      <c r="V72" s="44"/>
-      <c r="W72" s="44"/>
-      <c r="X72" s="44"/>
-      <c r="Y72" s="44"/>
-      <c r="Z72" s="44"/>
-      <c r="AA72" s="44"/>
-      <c r="AB72" s="45"/>
-    </row>
-    <row r="73" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="56"/>
-      <c r="B73" s="56"/>
-      <c r="C73" s="57"/>
-      <c r="D73" s="56"/>
-      <c r="E73" s="56"/>
-      <c r="F73" s="56"/>
-      <c r="G73" s="56"/>
-      <c r="H73" s="56"/>
-      <c r="I73" s="56"/>
-      <c r="J73" s="56"/>
-      <c r="K73" s="56"/>
-      <c r="L73" s="56"/>
-      <c r="M73" s="56"/>
-      <c r="N73" s="56"/>
-      <c r="O73" s="56"/>
-      <c r="P73" s="56"/>
-      <c r="Q73" s="56"/>
-      <c r="R73" s="56"/>
-      <c r="S73" s="56"/>
-      <c r="T73" s="56"/>
-      <c r="U73" s="56"/>
-      <c r="V73" s="56"/>
-      <c r="W73" s="56"/>
-      <c r="X73" s="56"/>
-      <c r="Y73" s="56"/>
-      <c r="Z73" s="56"/>
-      <c r="AA73" s="56"/>
-      <c r="AB73" s="56"/>
+      <c r="B73" s="44"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="44"/>
+      <c r="J73" s="44"/>
+      <c r="K73" s="44"/>
+      <c r="L73" s="44"/>
+      <c r="M73" s="44"/>
+      <c r="N73" s="44"/>
+      <c r="O73" s="44"/>
+      <c r="P73" s="44"/>
+      <c r="Q73" s="44"/>
+      <c r="R73" s="44"/>
+      <c r="S73" s="44"/>
+      <c r="T73" s="44"/>
+      <c r="U73" s="44"/>
+      <c r="V73" s="44"/>
+      <c r="W73" s="44"/>
+      <c r="X73" s="44"/>
+      <c r="Y73" s="44"/>
+      <c r="Z73" s="44"/>
+      <c r="AA73" s="44"/>
+      <c r="AB73" s="45"/>
     </row>
     <row r="74" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="58"/>
-      <c r="B74" s="58"/>
-      <c r="C74" s="59"/>
-      <c r="D74" s="58"/>
-      <c r="E74" s="58"/>
-      <c r="F74" s="58"/>
-      <c r="G74" s="58"/>
-      <c r="H74" s="58"/>
-      <c r="I74" s="58"/>
-      <c r="J74" s="58"/>
-      <c r="K74" s="58"/>
-      <c r="L74" s="58"/>
-      <c r="M74" s="58"/>
-      <c r="N74" s="58"/>
-      <c r="O74" s="58"/>
-      <c r="P74" s="58"/>
-      <c r="Q74" s="58"/>
-      <c r="R74" s="58"/>
-      <c r="S74" s="58"/>
-      <c r="T74" s="58"/>
-      <c r="U74" s="58"/>
-      <c r="V74" s="58"/>
-      <c r="W74" s="58"/>
-      <c r="X74" s="58"/>
-      <c r="Y74" s="58"/>
-      <c r="Z74" s="58"/>
-      <c r="AA74" s="58"/>
-      <c r="AB74" s="58"/>
+      <c r="A74" s="56"/>
+      <c r="B74" s="56"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="56"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="56"/>
+      <c r="G74" s="56"/>
+      <c r="H74" s="56"/>
+      <c r="I74" s="56"/>
+      <c r="J74" s="56"/>
+      <c r="K74" s="56"/>
+      <c r="L74" s="56"/>
+      <c r="M74" s="56"/>
+      <c r="N74" s="56"/>
+      <c r="O74" s="56"/>
+      <c r="P74" s="56"/>
+      <c r="Q74" s="56"/>
+      <c r="R74" s="56"/>
+      <c r="S74" s="56"/>
+      <c r="T74" s="56"/>
+      <c r="U74" s="56"/>
+      <c r="V74" s="56"/>
+      <c r="W74" s="56"/>
+      <c r="X74" s="56"/>
+      <c r="Y74" s="56"/>
+      <c r="Z74" s="56"/>
+      <c r="AA74" s="56"/>
+      <c r="AB74" s="56"/>
     </row>
     <row r="75" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="58"/>
@@ -35875,6 +36125,36 @@
       <c r="Z1045" s="58"/>
       <c r="AA1045" s="58"/>
       <c r="AB1045" s="58"/>
+    </row>
+    <row r="1046" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1046" s="58"/>
+      <c r="B1046" s="58"/>
+      <c r="C1046" s="59"/>
+      <c r="D1046" s="58"/>
+      <c r="E1046" s="58"/>
+      <c r="F1046" s="58"/>
+      <c r="G1046" s="58"/>
+      <c r="H1046" s="58"/>
+      <c r="I1046" s="58"/>
+      <c r="J1046" s="58"/>
+      <c r="K1046" s="58"/>
+      <c r="L1046" s="58"/>
+      <c r="M1046" s="58"/>
+      <c r="N1046" s="58"/>
+      <c r="O1046" s="58"/>
+      <c r="P1046" s="58"/>
+      <c r="Q1046" s="58"/>
+      <c r="R1046" s="58"/>
+      <c r="S1046" s="58"/>
+      <c r="T1046" s="58"/>
+      <c r="U1046" s="58"/>
+      <c r="V1046" s="58"/>
+      <c r="W1046" s="58"/>
+      <c r="X1046" s="58"/>
+      <c r="Y1046" s="58"/>
+      <c r="Z1046" s="58"/>
+      <c r="AA1046" s="58"/>
+      <c r="AB1046" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
refactor(register): add time of observation
</commit_message>
<xml_diff>
--- a/forms/app/register.xlsx
+++ b/forms/app/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Work/dccms/daily-register/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E1470B-9180-3A42-8B2C-A7991559C697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE828D73-1EC1-5C43-B2F4-ADC970AE7A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="186">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -597,6 +597,12 @@
   <si>
     <t>string</t>
   </si>
+  <si>
+    <t>n_x</t>
+  </si>
+  <si>
+    <t>Time of observation: ${datetime_of_observation}</t>
+  </si>
 </sst>
 </file>
 
@@ -926,7 +932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1106,6 +1112,11 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2444,10 +2455,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV1046"/>
+  <dimension ref="A1:IV1047"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6019,17 +6030,17 @@
       <c r="AB46" s="45"/>
     </row>
     <row r="47" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="42" t="s">
-        <v>123</v>
+      <c r="B47" s="89" t="s">
+        <v>184</v>
       </c>
-      <c r="C47" s="43" t="s">
-        <v>131</v>
+      <c r="C47" s="90" t="s">
+        <v>185</v>
       </c>
       <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
+      <c r="E47" s="42"/>
       <c r="F47" s="44"/>
       <c r="G47" s="44"/>
       <c r="H47" s="44"/>
@@ -6059,10 +6070,10 @@
         <v>23</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C48" s="43" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D48" s="44"/>
       <c r="E48" s="44"/>
@@ -6095,10 +6106,10 @@
         <v>23</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C49" s="43" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D49" s="44"/>
       <c r="E49" s="44"/>
@@ -6131,10 +6142,10 @@
         <v>23</v>
       </c>
       <c r="B50" s="42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C50" s="43" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D50" s="44"/>
       <c r="E50" s="44"/>
@@ -6167,10 +6178,10 @@
         <v>23</v>
       </c>
       <c r="B51" s="42" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C51" s="43" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D51" s="44"/>
       <c r="E51" s="44"/>
@@ -6200,10 +6211,14 @@
     </row>
     <row r="52" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="41" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="51"/>
+      <c r="B52" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>130</v>
+      </c>
       <c r="D52" s="44"/>
       <c r="E52" s="44"/>
       <c r="F52" s="44"/>
@@ -6231,7 +6246,9 @@
       <c r="AB52" s="45"/>
     </row>
     <row r="53" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="50"/>
+      <c r="A53" s="41" t="s">
+        <v>28</v>
+      </c>
       <c r="B53" s="44"/>
       <c r="C53" s="51"/>
       <c r="D53" s="44"/>
@@ -6261,17 +6278,11 @@
       <c r="AB53" s="45"/>
     </row>
     <row r="54" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="C54" s="51" t="s">
-        <v>82</v>
-      </c>
+      <c r="A54" s="50"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="51"/>
       <c r="D54" s="44"/>
-      <c r="E54" s="42"/>
+      <c r="E54" s="44"/>
       <c r="F54" s="44"/>
       <c r="G54" s="44"/>
       <c r="H54" s="44"/>
@@ -6298,16 +6309,16 @@
     </row>
     <row r="55" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
-      <c r="C55" s="43" t="s">
-        <v>134</v>
+      <c r="C55" s="51" t="s">
+        <v>82</v>
       </c>
       <c r="D55" s="44"/>
-      <c r="E55" s="44"/>
+      <c r="E55" s="42"/>
       <c r="F55" s="44"/>
       <c r="G55" s="44"/>
       <c r="H55" s="44"/>
@@ -6337,10 +6348,10 @@
         <v>23</v>
       </c>
       <c r="B56" s="42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C56" s="43" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="D56" s="44"/>
       <c r="E56" s="44"/>
@@ -6373,10 +6384,10 @@
         <v>23</v>
       </c>
       <c r="B57" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C57" s="43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D57" s="44"/>
       <c r="E57" s="44"/>
@@ -6409,10 +6420,10 @@
         <v>23</v>
       </c>
       <c r="B58" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C58" s="43" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="D58" s="44"/>
       <c r="E58" s="44"/>
@@ -6445,10 +6456,10 @@
         <v>23</v>
       </c>
       <c r="B59" s="42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D59" s="44"/>
       <c r="E59" s="44"/>
@@ -6481,10 +6492,10 @@
         <v>23</v>
       </c>
       <c r="B60" s="42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C60" s="43" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D60" s="44"/>
       <c r="E60" s="44"/>
@@ -6517,10 +6528,10 @@
         <v>23</v>
       </c>
       <c r="B61" s="42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="D61" s="44"/>
       <c r="E61" s="44"/>
@@ -6553,10 +6564,10 @@
         <v>23</v>
       </c>
       <c r="B62" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C62" s="43" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="D62" s="44"/>
       <c r="E62" s="44"/>
@@ -6589,10 +6600,10 @@
         <v>23</v>
       </c>
       <c r="B63" s="42" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C63" s="43" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D63" s="44"/>
       <c r="E63" s="44"/>
@@ -6625,10 +6636,10 @@
         <v>23</v>
       </c>
       <c r="B64" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C64" s="43" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D64" s="44"/>
       <c r="E64" s="44"/>
@@ -6661,10 +6672,10 @@
         <v>23</v>
       </c>
       <c r="B65" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C65" s="43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D65" s="44"/>
       <c r="E65" s="44"/>
@@ -6697,10 +6708,10 @@
         <v>23</v>
       </c>
       <c r="B66" s="42" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D66" s="44"/>
       <c r="E66" s="44"/>
@@ -6733,10 +6744,10 @@
         <v>23</v>
       </c>
       <c r="B67" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D67" s="44"/>
       <c r="E67" s="44"/>
@@ -6769,10 +6780,10 @@
         <v>23</v>
       </c>
       <c r="B68" s="42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C68" s="43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D68" s="44"/>
       <c r="E68" s="44"/>
@@ -6805,10 +6816,10 @@
         <v>23</v>
       </c>
       <c r="B69" s="42" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C69" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D69" s="44"/>
       <c r="E69" s="44"/>
@@ -6838,10 +6849,14 @@
     </row>
     <row r="70" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="41" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
-      <c r="B70" s="44"/>
-      <c r="C70" s="51"/>
+      <c r="B70" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" s="43" t="s">
+        <v>163</v>
+      </c>
       <c r="D70" s="44"/>
       <c r="E70" s="44"/>
       <c r="F70" s="44"/>
@@ -6869,7 +6884,9 @@
       <c r="AB70" s="45"/>
     </row>
     <row r="71" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="50"/>
+      <c r="A71" s="41" t="s">
+        <v>28</v>
+      </c>
       <c r="B71" s="44"/>
       <c r="C71" s="51"/>
       <c r="D71" s="44"/>
@@ -6898,133 +6915,133 @@
       <c r="AA71" s="44"/>
       <c r="AB71" s="45"/>
     </row>
-    <row r="72" spans="1:28" ht="35.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="52" t="s">
+    <row r="72" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="50"/>
+      <c r="B72" s="44"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="44"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="44"/>
+      <c r="J72" s="44"/>
+      <c r="K72" s="44"/>
+      <c r="L72" s="44"/>
+      <c r="M72" s="44"/>
+      <c r="N72" s="44"/>
+      <c r="O72" s="44"/>
+      <c r="P72" s="44"/>
+      <c r="Q72" s="44"/>
+      <c r="R72" s="44"/>
+      <c r="S72" s="44"/>
+      <c r="T72" s="44"/>
+      <c r="U72" s="44"/>
+      <c r="V72" s="44"/>
+      <c r="W72" s="44"/>
+      <c r="X72" s="44"/>
+      <c r="Y72" s="44"/>
+      <c r="Z72" s="44"/>
+      <c r="AA72" s="44"/>
+      <c r="AB72" s="45"/>
+    </row>
+    <row r="73" spans="1:28" ht="35.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B72" s="53" t="s">
+      <c r="B73" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="C72" s="47" t="s">
+      <c r="C73" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="D72" s="54"/>
-      <c r="E72" s="54"/>
-      <c r="F72" s="54"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="54"/>
-      <c r="I72" s="54"/>
-      <c r="J72" s="54"/>
-      <c r="K72" s="54"/>
-      <c r="L72" s="54"/>
-      <c r="M72" s="54"/>
-      <c r="N72" s="54"/>
-      <c r="O72" s="54"/>
-      <c r="P72" s="54"/>
-      <c r="Q72" s="54"/>
-      <c r="R72" s="54"/>
-      <c r="S72" s="54"/>
-      <c r="T72" s="54"/>
-      <c r="U72" s="54"/>
-      <c r="V72" s="54"/>
-      <c r="W72" s="54"/>
-      <c r="X72" s="54"/>
-      <c r="Y72" s="54"/>
-      <c r="Z72" s="54"/>
-      <c r="AA72" s="54"/>
-      <c r="AB72" s="55"/>
-    </row>
-    <row r="73" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="41" t="s">
+      <c r="D73" s="54"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="54"/>
+      <c r="G73" s="54"/>
+      <c r="H73" s="54"/>
+      <c r="I73" s="54"/>
+      <c r="J73" s="54"/>
+      <c r="K73" s="54"/>
+      <c r="L73" s="54"/>
+      <c r="M73" s="54"/>
+      <c r="N73" s="54"/>
+      <c r="O73" s="54"/>
+      <c r="P73" s="54"/>
+      <c r="Q73" s="54"/>
+      <c r="R73" s="54"/>
+      <c r="S73" s="54"/>
+      <c r="T73" s="54"/>
+      <c r="U73" s="54"/>
+      <c r="V73" s="54"/>
+      <c r="W73" s="54"/>
+      <c r="X73" s="54"/>
+      <c r="Y73" s="54"/>
+      <c r="Z73" s="54"/>
+      <c r="AA73" s="54"/>
+      <c r="AB73" s="55"/>
+    </row>
+    <row r="74" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B73" s="44"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="44"/>
-      <c r="E73" s="44"/>
-      <c r="F73" s="44"/>
-      <c r="G73" s="44"/>
-      <c r="H73" s="44"/>
-      <c r="I73" s="44"/>
-      <c r="J73" s="44"/>
-      <c r="K73" s="44"/>
-      <c r="L73" s="44"/>
-      <c r="M73" s="44"/>
-      <c r="N73" s="44"/>
-      <c r="O73" s="44"/>
-      <c r="P73" s="44"/>
-      <c r="Q73" s="44"/>
-      <c r="R73" s="44"/>
-      <c r="S73" s="44"/>
-      <c r="T73" s="44"/>
-      <c r="U73" s="44"/>
-      <c r="V73" s="44"/>
-      <c r="W73" s="44"/>
-      <c r="X73" s="44"/>
-      <c r="Y73" s="44"/>
-      <c r="Z73" s="44"/>
-      <c r="AA73" s="44"/>
-      <c r="AB73" s="45"/>
-    </row>
-    <row r="74" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="56"/>
-      <c r="B74" s="56"/>
-      <c r="C74" s="57"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56"/>
-      <c r="G74" s="56"/>
-      <c r="H74" s="56"/>
-      <c r="I74" s="56"/>
-      <c r="J74" s="56"/>
-      <c r="K74" s="56"/>
-      <c r="L74" s="56"/>
-      <c r="M74" s="56"/>
-      <c r="N74" s="56"/>
-      <c r="O74" s="56"/>
-      <c r="P74" s="56"/>
-      <c r="Q74" s="56"/>
-      <c r="R74" s="56"/>
-      <c r="S74" s="56"/>
-      <c r="T74" s="56"/>
-      <c r="U74" s="56"/>
-      <c r="V74" s="56"/>
-      <c r="W74" s="56"/>
-      <c r="X74" s="56"/>
-      <c r="Y74" s="56"/>
-      <c r="Z74" s="56"/>
-      <c r="AA74" s="56"/>
-      <c r="AB74" s="56"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="51"/>
+      <c r="D74" s="44"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="44"/>
+      <c r="G74" s="44"/>
+      <c r="H74" s="44"/>
+      <c r="I74" s="44"/>
+      <c r="J74" s="44"/>
+      <c r="K74" s="44"/>
+      <c r="L74" s="44"/>
+      <c r="M74" s="44"/>
+      <c r="N74" s="44"/>
+      <c r="O74" s="44"/>
+      <c r="P74" s="44"/>
+      <c r="Q74" s="44"/>
+      <c r="R74" s="44"/>
+      <c r="S74" s="44"/>
+      <c r="T74" s="44"/>
+      <c r="U74" s="44"/>
+      <c r="V74" s="44"/>
+      <c r="W74" s="44"/>
+      <c r="X74" s="44"/>
+      <c r="Y74" s="44"/>
+      <c r="Z74" s="44"/>
+      <c r="AA74" s="44"/>
+      <c r="AB74" s="45"/>
     </row>
     <row r="75" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="58"/>
-      <c r="B75" s="58"/>
-      <c r="C75" s="59"/>
-      <c r="D75" s="58"/>
-      <c r="E75" s="58"/>
-      <c r="F75" s="58"/>
-      <c r="G75" s="58"/>
-      <c r="H75" s="58"/>
-      <c r="I75" s="58"/>
-      <c r="J75" s="58"/>
-      <c r="K75" s="58"/>
-      <c r="L75" s="58"/>
-      <c r="M75" s="58"/>
-      <c r="N75" s="58"/>
-      <c r="O75" s="58"/>
-      <c r="P75" s="58"/>
-      <c r="Q75" s="58"/>
-      <c r="R75" s="58"/>
-      <c r="S75" s="58"/>
-      <c r="T75" s="58"/>
-      <c r="U75" s="58"/>
-      <c r="V75" s="58"/>
-      <c r="W75" s="58"/>
-      <c r="X75" s="58"/>
-      <c r="Y75" s="58"/>
-      <c r="Z75" s="58"/>
-      <c r="AA75" s="58"/>
-      <c r="AB75" s="58"/>
+      <c r="A75" s="56"/>
+      <c r="B75" s="56"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="56"/>
+      <c r="E75" s="56"/>
+      <c r="F75" s="56"/>
+      <c r="G75" s="56"/>
+      <c r="H75" s="56"/>
+      <c r="I75" s="56"/>
+      <c r="J75" s="56"/>
+      <c r="K75" s="56"/>
+      <c r="L75" s="56"/>
+      <c r="M75" s="56"/>
+      <c r="N75" s="56"/>
+      <c r="O75" s="56"/>
+      <c r="P75" s="56"/>
+      <c r="Q75" s="56"/>
+      <c r="R75" s="56"/>
+      <c r="S75" s="56"/>
+      <c r="T75" s="56"/>
+      <c r="U75" s="56"/>
+      <c r="V75" s="56"/>
+      <c r="W75" s="56"/>
+      <c r="X75" s="56"/>
+      <c r="Y75" s="56"/>
+      <c r="Z75" s="56"/>
+      <c r="AA75" s="56"/>
+      <c r="AB75" s="56"/>
     </row>
     <row r="76" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="58"/>
@@ -36155,6 +36172,36 @@
       <c r="Z1046" s="58"/>
       <c r="AA1046" s="58"/>
       <c r="AB1046" s="58"/>
+    </row>
+    <row r="1047" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1047" s="58"/>
+      <c r="B1047" s="58"/>
+      <c r="C1047" s="59"/>
+      <c r="D1047" s="58"/>
+      <c r="E1047" s="58"/>
+      <c r="F1047" s="58"/>
+      <c r="G1047" s="58"/>
+      <c r="H1047" s="58"/>
+      <c r="I1047" s="58"/>
+      <c r="J1047" s="58"/>
+      <c r="K1047" s="58"/>
+      <c r="L1047" s="58"/>
+      <c r="M1047" s="58"/>
+      <c r="N1047" s="58"/>
+      <c r="O1047" s="58"/>
+      <c r="P1047" s="58"/>
+      <c r="Q1047" s="58"/>
+      <c r="R1047" s="58"/>
+      <c r="S1047" s="58"/>
+      <c r="T1047" s="58"/>
+      <c r="U1047" s="58"/>
+      <c r="V1047" s="58"/>
+      <c r="W1047" s="58"/>
+      <c r="X1047" s="58"/>
+      <c r="Y1047" s="58"/>
+      <c r="Z1047" s="58"/>
+      <c r="AA1047" s="58"/>
+      <c r="AB1047" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
refactor(register): refactor weather types
- refactored weather types
- present weather now accepts integers between 1 and 99
- past weather now accepts integers between 1 and 9
</commit_message>
<xml_diff>
--- a/forms/app/register.xlsx
+++ b/forms/app/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Work/dccms/daily-register/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9991FBE0-2BED-1546-9374-295FCF39B9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F0B50B-D4AC-3B47-A168-7D4E4AB6739B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="226">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -62,6 +62,7 @@
         <sz val="12"/>
         <color indexed="11"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>survey</t>
     </r>
@@ -239,9 +240,6 @@
   </si>
   <si>
     <t>past_weather</t>
-  </si>
-  <si>
-    <t>select one weather_types</t>
   </si>
   <si>
     <t>Present weather</t>
@@ -714,6 +712,18 @@
   <si>
     <t>selected(${reporting_on}, 'earth_temperature_at_1_2')</t>
   </si>
+  <si>
+    <t>. &gt;= 1 and . &lt;= 99</t>
+  </si>
+  <si>
+    <t>. &gt;= 1 and . &lt;= 9</t>
+  </si>
+  <si>
+    <t>Present weather can only be between 1 and 99</t>
+  </si>
+  <si>
+    <t>Past weather can only be between 1 and 9</t>
+  </si>
 </sst>
 </file>
 
@@ -729,23 +739,27 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1088,7 +1102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1303,10 +1317,6 @@
     <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1315,10 +1325,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1329,6 +1338,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2519,11 +2532,11 @@
     </row>
     <row r="3" spans="1:5" ht="0" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2668,8 +2681,8 @@
   </sheetPr>
   <dimension ref="A1:IV1043"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3009,13 +3022,13 @@
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" s="64" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="65" t="s">
         <v>173</v>
-      </c>
-      <c r="C3" s="65" t="s">
-        <v>174</v>
       </c>
       <c r="D3" s="65"/>
       <c r="E3" s="66"/>
@@ -3025,7 +3038,7 @@
       <c r="I3" s="74"/>
       <c r="J3" s="67"/>
       <c r="K3" s="68" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L3" s="68"/>
       <c r="M3" s="69"/>
@@ -4760,10 +4773,10 @@
         <v>21</v>
       </c>
       <c r="B14" s="96" t="s">
-        <v>194</v>
-      </c>
-      <c r="C14" s="100" t="s">
         <v>193</v>
+      </c>
+      <c r="C14" s="98" t="s">
+        <v>192</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -4833,13 +4846,13 @@
     </row>
     <row r="16" spans="1:256" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="76" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="76" t="s">
+      <c r="C16" s="77" t="s">
         <v>171</v>
-      </c>
-      <c r="C16" s="77" t="s">
-        <v>172</v>
       </c>
       <c r="D16" s="78" t="s">
         <v>26</v>
@@ -4870,21 +4883,21 @@
       <c r="AB16" s="38"/>
     </row>
     <row r="17" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="101" t="s">
-        <v>198</v>
+      <c r="A17" s="99" t="s">
+        <v>197</v>
       </c>
       <c r="B17" s="96" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="98" t="s">
         <v>195</v>
-      </c>
-      <c r="C17" s="100" t="s">
-        <v>196</v>
       </c>
       <c r="D17" s="82" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="96" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
@@ -4925,7 +4938,7 @@
         <v>26</v>
       </c>
       <c r="E18" s="82" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="31"/>
@@ -4934,7 +4947,7 @@
       </c>
       <c r="I18" s="87"/>
       <c r="J18" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
@@ -4969,7 +4982,7 @@
         <v>26</v>
       </c>
       <c r="E19" s="82" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F19" s="31"/>
       <c r="G19" s="31"/>
@@ -5003,13 +5016,13 @@
         <v>62</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D20" s="29" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="82" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
@@ -5018,7 +5031,7 @@
       </c>
       <c r="I20" s="89"/>
       <c r="J20" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K20" s="31"/>
       <c r="L20" s="31"/>
@@ -5040,25 +5053,29 @@
       <c r="AB20" s="32"/>
     </row>
     <row r="21" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="28" t="s">
-        <v>65</v>
+      <c r="A21" s="99" t="s">
+        <v>29</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>63</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>26</v>
       </c>
       <c r="E21" s="82" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F21" s="31"/>
       <c r="G21" s="29"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="87"/>
+      <c r="H21" s="82" t="s">
+        <v>222</v>
+      </c>
+      <c r="I21" s="90" t="s">
+        <v>224</v>
+      </c>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
       <c r="L21" s="29"/>
@@ -5080,25 +5097,29 @@
       <c r="AB21" s="32"/>
     </row>
     <row r="22" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="101" t="s">
+      <c r="A22" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="99" t="s">
         <v>64</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="29" t="s">
         <v>26</v>
       </c>
       <c r="E22" s="82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F22" s="31"/>
       <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="87"/>
+      <c r="H22" s="82" t="s">
+        <v>223</v>
+      </c>
+      <c r="I22" s="90" t="s">
+        <v>225</v>
+      </c>
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
@@ -5124,25 +5145,25 @@
         <v>29</v>
       </c>
       <c r="B23" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>79</v>
-      </c>
-      <c r="C23" s="35" t="s">
-        <v>80</v>
       </c>
       <c r="D23" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E23" s="82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="31"/>
       <c r="H23" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I23" s="87"/>
       <c r="J23" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
@@ -5168,16 +5189,16 @@
         <v>55</v>
       </c>
       <c r="B24" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="35" t="s">
         <v>86</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>87</v>
       </c>
       <c r="D24" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="82" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="31"/>
@@ -5186,7 +5207,7 @@
       </c>
       <c r="I24" s="87"/>
       <c r="J24" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
@@ -5212,27 +5233,27 @@
         <v>55</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="77" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D25" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="82" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="31"/>
       <c r="H25" s="82" t="s">
+        <v>178</v>
+      </c>
+      <c r="I25" s="90" t="s">
         <v>179</v>
       </c>
-      <c r="I25" s="90" t="s">
-        <v>180</v>
-      </c>
       <c r="J25" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
@@ -5258,27 +5279,27 @@
         <v>55</v>
       </c>
       <c r="B26" s="76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="35" t="s">
         <v>90</v>
-      </c>
-      <c r="C26" s="35" t="s">
-        <v>91</v>
       </c>
       <c r="D26" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E26" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="31"/>
       <c r="H26" s="82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I26" s="90" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J26" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
@@ -5304,27 +5325,27 @@
         <v>55</v>
       </c>
       <c r="B27" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="35" t="s">
         <v>93</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>94</v>
       </c>
       <c r="D27" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="31"/>
       <c r="H27" s="82" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I27" s="90" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J27" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>
@@ -5350,27 +5371,27 @@
         <v>55</v>
       </c>
       <c r="B28" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="35" t="s">
         <v>95</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>96</v>
       </c>
       <c r="D28" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E28" s="82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="31"/>
       <c r="H28" s="82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I28" s="90" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J28" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K28" s="31"/>
       <c r="L28" s="31"/>
@@ -5396,27 +5417,27 @@
         <v>55</v>
       </c>
       <c r="B29" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="35" t="s">
         <v>97</v>
-      </c>
-      <c r="C29" s="35" t="s">
-        <v>98</v>
       </c>
       <c r="D29" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E29" s="82" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F29" s="29"/>
       <c r="G29" s="31"/>
       <c r="H29" s="82" t="s">
+        <v>189</v>
+      </c>
+      <c r="I29" s="90" t="s">
         <v>190</v>
       </c>
-      <c r="I29" s="90" t="s">
-        <v>191</v>
-      </c>
       <c r="J29" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K29" s="31"/>
       <c r="L29" s="31"/>
@@ -5442,16 +5463,16 @@
         <v>55</v>
       </c>
       <c r="B30" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="35" t="s">
         <v>99</v>
-      </c>
-      <c r="C30" s="35" t="s">
-        <v>100</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E30" s="82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F30" s="29"/>
       <c r="G30" s="31"/>
@@ -5460,7 +5481,7 @@
       </c>
       <c r="I30" s="87"/>
       <c r="J30" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K30" s="31"/>
       <c r="L30" s="31"/>
@@ -5483,19 +5504,19 @@
     </row>
     <row r="31" spans="1:28" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31" s="76" t="s">
         <v>181</v>
       </c>
-      <c r="B31" s="76" t="s">
+      <c r="C31" s="77" t="s">
         <v>182</v>
-      </c>
-      <c r="C31" s="77" t="s">
-        <v>183</v>
       </c>
       <c r="D31" s="95" t="s">
         <v>26</v>
       </c>
       <c r="E31" s="96" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F31" s="29"/>
       <c r="G31" s="31"/>
@@ -5526,27 +5547,27 @@
         <v>55</v>
       </c>
       <c r="B32" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="35" t="s">
         <v>101</v>
-      </c>
-      <c r="C32" s="35" t="s">
-        <v>102</v>
       </c>
       <c r="D32" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F32" s="29"/>
       <c r="G32" s="31"/>
       <c r="H32" s="82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I32" s="97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J32" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K32" s="31"/>
       <c r="L32" s="31"/>
@@ -5572,27 +5593,27 @@
         <v>55</v>
       </c>
       <c r="B33" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="35" t="s">
         <v>103</v>
-      </c>
-      <c r="C33" s="35" t="s">
-        <v>104</v>
       </c>
       <c r="D33" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E33" s="82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F33" s="29"/>
       <c r="G33" s="31"/>
       <c r="H33" s="82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I33" s="97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J33" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K33" s="31"/>
       <c r="L33" s="31"/>
@@ -5618,27 +5639,27 @@
         <v>55</v>
       </c>
       <c r="B34" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="35" t="s">
         <v>105</v>
-      </c>
-      <c r="C34" s="35" t="s">
-        <v>106</v>
       </c>
       <c r="D34" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E34" s="82" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F34" s="29"/>
       <c r="G34" s="31"/>
       <c r="H34" s="82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I34" s="97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J34" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K34" s="31"/>
       <c r="L34" s="31"/>
@@ -5664,27 +5685,27 @@
         <v>55</v>
       </c>
       <c r="B35" s="76" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D35" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E35" s="82" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F35" s="29"/>
       <c r="G35" s="31"/>
       <c r="H35" s="82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I35" s="97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J35" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K35" s="31"/>
       <c r="L35" s="31"/>
@@ -5710,27 +5731,27 @@
         <v>55</v>
       </c>
       <c r="B36" s="76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D36" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E36" s="82" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F36" s="29"/>
       <c r="G36" s="31"/>
       <c r="H36" s="82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I36" s="97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J36" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K36" s="31"/>
       <c r="L36" s="31"/>
@@ -5756,27 +5777,27 @@
         <v>55</v>
       </c>
       <c r="B37" s="76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D37" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F37" s="29"/>
       <c r="G37" s="31"/>
       <c r="H37" s="82" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I37" s="97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J37" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K37" s="31"/>
       <c r="L37" s="31"/>
@@ -5802,23 +5823,23 @@
         <v>55</v>
       </c>
       <c r="B38" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="35" t="s">
         <v>110</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>111</v>
       </c>
       <c r="D38" s="37" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="82" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="31"/>
       <c r="H38" s="31"/>
       <c r="I38" s="87"/>
       <c r="J38" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K38" s="31"/>
       <c r="L38" s="31"/>
@@ -6042,10 +6063,10 @@
         <v>21</v>
       </c>
       <c r="B45" s="80" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C45" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D45" s="43"/>
       <c r="E45" s="41"/>
@@ -6078,10 +6099,10 @@
         <v>23</v>
       </c>
       <c r="B46" s="80" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="81" t="s">
         <v>177</v>
-      </c>
-      <c r="C46" s="81" t="s">
-        <v>178</v>
       </c>
       <c r="D46" s="43"/>
       <c r="E46" s="41"/>
@@ -6114,14 +6135,14 @@
         <v>23</v>
       </c>
       <c r="B47" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C47" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D47" s="43"/>
       <c r="E47" s="82" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F47" s="43"/>
       <c r="G47" s="43"/>
@@ -6152,14 +6173,14 @@
         <v>23</v>
       </c>
       <c r="B48" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="42" t="s">
         <v>117</v>
-      </c>
-      <c r="C48" s="42" t="s">
-        <v>118</v>
       </c>
       <c r="D48" s="43"/>
       <c r="E48" s="82" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F48" s="43"/>
       <c r="G48" s="43"/>
@@ -6190,14 +6211,14 @@
         <v>23</v>
       </c>
       <c r="B49" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D49" s="43"/>
       <c r="E49" s="82" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F49" s="43"/>
       <c r="G49" s="43"/>
@@ -6228,14 +6249,14 @@
         <v>23</v>
       </c>
       <c r="B50" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="42" t="s">
         <v>120</v>
-      </c>
-      <c r="C50" s="42" t="s">
-        <v>121</v>
       </c>
       <c r="D50" s="43"/>
       <c r="E50" s="82" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F50" s="43"/>
       <c r="G50" s="43"/>
@@ -6266,14 +6287,14 @@
         <v>23</v>
       </c>
       <c r="B51" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="42" t="s">
         <v>122</v>
-      </c>
-      <c r="C51" s="42" t="s">
-        <v>123</v>
       </c>
       <c r="D51" s="43"/>
       <c r="E51" s="82" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F51" s="43"/>
       <c r="G51" s="43"/>
@@ -6304,14 +6325,14 @@
         <v>23</v>
       </c>
       <c r="B52" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C52" s="42" t="s">
         <v>126</v>
-      </c>
-      <c r="C52" s="42" t="s">
-        <v>127</v>
       </c>
       <c r="D52" s="43"/>
       <c r="E52" s="82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F52" s="43"/>
       <c r="G52" s="43"/>
@@ -6342,14 +6363,14 @@
         <v>23</v>
       </c>
       <c r="B53" s="41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D53" s="43"/>
       <c r="E53" s="82" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F53" s="43"/>
       <c r="G53" s="43"/>
@@ -6380,14 +6401,14 @@
         <v>23</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D54" s="43"/>
       <c r="E54" s="82" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F54" s="43"/>
       <c r="G54" s="43"/>
@@ -6418,14 +6439,14 @@
         <v>23</v>
       </c>
       <c r="B55" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="42" t="s">
         <v>130</v>
-      </c>
-      <c r="C55" s="42" t="s">
-        <v>131</v>
       </c>
       <c r="D55" s="43"/>
       <c r="E55" s="82" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F55" s="43"/>
       <c r="G55" s="43"/>
@@ -6456,14 +6477,14 @@
         <v>23</v>
       </c>
       <c r="B56" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="42" t="s">
         <v>132</v>
-      </c>
-      <c r="C56" s="42" t="s">
-        <v>133</v>
       </c>
       <c r="D56" s="43"/>
       <c r="E56" s="82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F56" s="43"/>
       <c r="G56" s="43"/>
@@ -6494,14 +6515,14 @@
         <v>23</v>
       </c>
       <c r="B57" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" s="42" t="s">
         <v>134</v>
-      </c>
-      <c r="C57" s="42" t="s">
-        <v>135</v>
       </c>
       <c r="D57" s="43"/>
       <c r="E57" s="82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F57" s="43"/>
       <c r="G57" s="43"/>
@@ -6532,14 +6553,14 @@
         <v>23</v>
       </c>
       <c r="B58" s="41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C58" s="42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D58" s="43"/>
       <c r="E58" s="82" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F58" s="43"/>
       <c r="G58" s="43"/>
@@ -6570,14 +6591,14 @@
         <v>23</v>
       </c>
       <c r="B59" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59" s="42" t="s">
         <v>137</v>
-      </c>
-      <c r="C59" s="42" t="s">
-        <v>138</v>
       </c>
       <c r="D59" s="43"/>
       <c r="E59" s="82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F59" s="43"/>
       <c r="G59" s="43"/>
@@ -6608,14 +6629,14 @@
         <v>23</v>
       </c>
       <c r="B60" s="41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C60" s="42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D60" s="43"/>
       <c r="E60" s="82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F60" s="43"/>
       <c r="G60" s="43"/>
@@ -6646,14 +6667,14 @@
         <v>23</v>
       </c>
       <c r="B61" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C61" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D61" s="43"/>
       <c r="E61" s="82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F61" s="43"/>
       <c r="G61" s="43"/>
@@ -6684,14 +6705,14 @@
         <v>23</v>
       </c>
       <c r="B62" s="41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C62" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D62" s="43"/>
       <c r="E62" s="82" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F62" s="43"/>
       <c r="G62" s="43"/>
@@ -6722,14 +6743,14 @@
         <v>23</v>
       </c>
       <c r="B63" s="41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D63" s="43"/>
       <c r="E63" s="82" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F63" s="43"/>
       <c r="G63" s="43"/>
@@ -6760,14 +6781,14 @@
         <v>23</v>
       </c>
       <c r="B64" s="41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C64" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D64" s="43"/>
       <c r="E64" s="82" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F64" s="43"/>
       <c r="G64" s="43"/>
@@ -6798,14 +6819,14 @@
         <v>23</v>
       </c>
       <c r="B65" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C65" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D65" s="43"/>
       <c r="E65" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F65" s="43"/>
       <c r="G65" s="43"/>
@@ -6836,14 +6857,14 @@
         <v>23</v>
       </c>
       <c r="B66" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="C66" s="42" t="s">
         <v>155</v>
-      </c>
-      <c r="C66" s="42" t="s">
-        <v>156</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="82" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F66" s="43"/>
       <c r="G66" s="43"/>
@@ -6936,10 +6957,10 @@
         <v>23</v>
       </c>
       <c r="B69" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C69" s="46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D69" s="53"/>
       <c r="E69" s="53"/>
@@ -36257,10 +36278,10 @@
         <v>59</v>
       </c>
       <c r="B2" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="57" t="s">
         <v>157</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>158</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
@@ -36291,10 +36312,10 @@
         <v>59</v>
       </c>
       <c r="B3" s="57" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="57" t="s">
         <v>159</v>
-      </c>
-      <c r="C3" s="57" t="s">
-        <v>160</v>
       </c>
       <c r="D3" s="57"/>
       <c r="E3" s="57"/>
@@ -36325,10 +36346,10 @@
         <v>59</v>
       </c>
       <c r="B4" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="57" t="s">
         <v>161</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>162</v>
       </c>
       <c r="D4" s="57"/>
       <c r="E4" s="57"/>
@@ -36359,10 +36380,10 @@
         <v>59</v>
       </c>
       <c r="B5" s="57" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="57" t="s">
         <v>163</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>164</v>
       </c>
       <c r="D5" s="57"/>
       <c r="E5" s="57"/>
@@ -36393,10 +36414,10 @@
         <v>59</v>
       </c>
       <c r="B6" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="57" t="s">
         <v>165</v>
-      </c>
-      <c r="C6" s="57" t="s">
-        <v>166</v>
       </c>
       <c r="D6" s="57"/>
       <c r="E6" s="57"/>
@@ -36452,13 +36473,13 @@
     </row>
     <row r="8" spans="1:26" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="C8" s="61" t="s">
         <v>69</v>
-      </c>
-      <c r="C8" s="61" t="s">
-        <v>70</v>
       </c>
       <c r="D8" s="57"/>
       <c r="E8" s="57"/>
@@ -36486,13 +36507,13 @@
     </row>
     <row r="9" spans="1:26" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="61" t="s">
         <v>71</v>
-      </c>
-      <c r="C9" s="61" t="s">
-        <v>72</v>
       </c>
       <c r="D9" s="57"/>
       <c r="E9" s="57"/>
@@ -36520,13 +36541,13 @@
     </row>
     <row r="10" spans="1:26" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="61" t="s">
         <v>73</v>
-      </c>
-      <c r="C10" s="61" t="s">
-        <v>74</v>
       </c>
       <c r="D10" s="57"/>
       <c r="E10" s="57"/>
@@ -36554,13 +36575,13 @@
     </row>
     <row r="11" spans="1:26" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="61" t="s">
         <v>75</v>
-      </c>
-      <c r="C11" s="61" t="s">
-        <v>76</v>
       </c>
       <c r="D11" s="57"/>
       <c r="E11" s="57"/>
@@ -36587,746 +36608,746 @@
       <c r="Z11" s="57"/>
     </row>
     <row r="12" spans="1:26" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="102" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="102" t="s">
+      <c r="A12" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="100" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="101"/>
+      <c r="E12" s="101"/>
+      <c r="F12" s="101"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="101"/>
+      <c r="L12" s="101"/>
+      <c r="M12" s="101"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="101"/>
+      <c r="P12" s="101"/>
+      <c r="Q12" s="101"/>
+      <c r="R12" s="101"/>
+      <c r="S12" s="101"/>
+      <c r="T12" s="101"/>
+      <c r="U12" s="101"/>
+      <c r="V12" s="101"/>
+      <c r="W12" s="101"/>
+      <c r="X12" s="101"/>
+      <c r="Y12" s="101"/>
+      <c r="Z12" s="101"/>
+    </row>
+    <row r="13" spans="1:26" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="102"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="103"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="103"/>
+      <c r="K13" s="103"/>
+      <c r="L13" s="103"/>
+      <c r="M13" s="103"/>
+      <c r="N13" s="103"/>
+      <c r="O13" s="103"/>
+      <c r="P13" s="103"/>
+      <c r="Q13" s="103"/>
+      <c r="R13" s="103"/>
+      <c r="S13" s="103"/>
+      <c r="T13" s="103"/>
+      <c r="U13" s="103"/>
+      <c r="V13" s="103"/>
+      <c r="W13" s="103"/>
+      <c r="X13" s="103"/>
+      <c r="Y13" s="103"/>
+      <c r="Z13" s="103"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="105" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
+      <c r="G14" s="104"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="104"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="104"/>
+      <c r="L14" s="104"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="104"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
+      <c r="U14" s="104"/>
+      <c r="V14" s="104"/>
+      <c r="W14" s="104"/>
+      <c r="X14" s="104"/>
+      <c r="Y14" s="104"/>
+      <c r="Z14" s="104"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="105" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
+      <c r="G15" s="104"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="104"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
+      <c r="M15" s="104"/>
+      <c r="N15" s="104"/>
+      <c r="O15" s="104"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="104"/>
+      <c r="R15" s="104"/>
+      <c r="S15" s="104"/>
+      <c r="T15" s="104"/>
+      <c r="U15" s="104"/>
+      <c r="V15" s="104"/>
+      <c r="W15" s="104"/>
+      <c r="X15" s="104"/>
+      <c r="Y15" s="104"/>
+      <c r="Z15" s="104"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" s="109" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="105" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="104"/>
+      <c r="H16" s="104"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="104"/>
+      <c r="L16" s="104"/>
+      <c r="M16" s="104"/>
+      <c r="N16" s="104"/>
+      <c r="O16" s="104"/>
+      <c r="P16" s="104"/>
+      <c r="Q16" s="104"/>
+      <c r="R16" s="104"/>
+      <c r="S16" s="104"/>
+      <c r="T16" s="104"/>
+      <c r="U16" s="104"/>
+      <c r="V16" s="104"/>
+      <c r="W16" s="104"/>
+      <c r="X16" s="104"/>
+      <c r="Y16" s="104"/>
+      <c r="Z16" s="104"/>
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="109" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="105" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="104"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="104"/>
+      <c r="I17" s="104"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="104"/>
+      <c r="L17" s="104"/>
+      <c r="M17" s="104"/>
+      <c r="N17" s="104"/>
+      <c r="O17" s="104"/>
+      <c r="P17" s="104"/>
+      <c r="Q17" s="104"/>
+      <c r="R17" s="104"/>
+      <c r="S17" s="104"/>
+      <c r="T17" s="104"/>
+      <c r="U17" s="104"/>
+      <c r="V17" s="104"/>
+      <c r="W17" s="104"/>
+      <c r="X17" s="104"/>
+      <c r="Y17" s="104"/>
+      <c r="Z17" s="104"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="109" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="104"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="104"/>
+      <c r="L18" s="104"/>
+      <c r="M18" s="104"/>
+      <c r="N18" s="104"/>
+      <c r="O18" s="104"/>
+      <c r="P18" s="104"/>
+      <c r="Q18" s="104"/>
+      <c r="R18" s="104"/>
+      <c r="S18" s="104"/>
+      <c r="T18" s="104"/>
+      <c r="U18" s="104"/>
+      <c r="V18" s="104"/>
+      <c r="W18" s="104"/>
+      <c r="X18" s="104"/>
+      <c r="Y18" s="104"/>
+      <c r="Z18" s="104"/>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="102" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
-      <c r="L12" s="103"/>
-      <c r="M12" s="103"/>
-      <c r="N12" s="103"/>
-      <c r="O12" s="103"/>
-      <c r="P12" s="103"/>
-      <c r="Q12" s="103"/>
-      <c r="R12" s="103"/>
-      <c r="S12" s="103"/>
-      <c r="T12" s="103"/>
-      <c r="U12" s="103"/>
-      <c r="V12" s="103"/>
-      <c r="W12" s="103"/>
-      <c r="X12" s="103"/>
-      <c r="Y12" s="103"/>
-      <c r="Z12" s="103"/>
-    </row>
-    <row r="13" spans="1:26" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="104"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="105"/>
-      <c r="O13" s="105"/>
-      <c r="P13" s="105"/>
-      <c r="Q13" s="105"/>
-      <c r="R13" s="105"/>
-      <c r="S13" s="105"/>
-      <c r="T13" s="105"/>
-      <c r="U13" s="105"/>
-      <c r="V13" s="105"/>
-      <c r="W13" s="105"/>
-      <c r="X13" s="105"/>
-      <c r="Y13" s="105"/>
-      <c r="Z13" s="105"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B14" s="108" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="108" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="107"/>
-      <c r="E14" s="107"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="107"/>
-      <c r="H14" s="107"/>
-      <c r="I14" s="107"/>
-      <c r="J14" s="107"/>
-      <c r="K14" s="107"/>
-      <c r="L14" s="107"/>
-      <c r="M14" s="107"/>
-      <c r="N14" s="107"/>
-      <c r="O14" s="107"/>
-      <c r="P14" s="107"/>
-      <c r="Q14" s="107"/>
-      <c r="R14" s="107"/>
-      <c r="S14" s="107"/>
-      <c r="T14" s="107"/>
-      <c r="U14" s="107"/>
-      <c r="V14" s="107"/>
-      <c r="W14" s="107"/>
-      <c r="X14" s="107"/>
-      <c r="Y14" s="107"/>
-      <c r="Z14" s="107"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B15" s="108" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="108" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="107"/>
-      <c r="E15" s="107"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="107"/>
-      <c r="I15" s="107"/>
-      <c r="J15" s="107"/>
-      <c r="K15" s="107"/>
-      <c r="L15" s="107"/>
-      <c r="M15" s="107"/>
-      <c r="N15" s="107"/>
-      <c r="O15" s="107"/>
-      <c r="P15" s="107"/>
-      <c r="Q15" s="107"/>
-      <c r="R15" s="107"/>
-      <c r="S15" s="107"/>
-      <c r="T15" s="107"/>
-      <c r="U15" s="107"/>
-      <c r="V15" s="107"/>
-      <c r="W15" s="107"/>
-      <c r="X15" s="107"/>
-      <c r="Y15" s="107"/>
-      <c r="Z15" s="107"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B16" s="112" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="108" t="s">
+      <c r="C19" s="105" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="104"/>
+      <c r="M19" s="104"/>
+      <c r="N19" s="104"/>
+      <c r="O19" s="104"/>
+      <c r="P19" s="104"/>
+      <c r="Q19" s="104"/>
+      <c r="R19" s="104"/>
+      <c r="S19" s="104"/>
+      <c r="T19" s="104"/>
+      <c r="U19" s="104"/>
+      <c r="V19" s="104"/>
+      <c r="W19" s="104"/>
+      <c r="X19" s="104"/>
+      <c r="Y19" s="104"/>
+      <c r="Z19" s="104"/>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B20" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="107"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="107"/>
-      <c r="G16" s="107"/>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107"/>
-      <c r="J16" s="107"/>
-      <c r="K16" s="107"/>
-      <c r="L16" s="107"/>
-      <c r="M16" s="107"/>
-      <c r="N16" s="107"/>
-      <c r="O16" s="107"/>
-      <c r="P16" s="107"/>
-      <c r="Q16" s="107"/>
-      <c r="R16" s="107"/>
-      <c r="S16" s="107"/>
-      <c r="T16" s="107"/>
-      <c r="U16" s="107"/>
-      <c r="V16" s="107"/>
-      <c r="W16" s="107"/>
-      <c r="X16" s="107"/>
-      <c r="Y16" s="107"/>
-      <c r="Z16" s="107"/>
-    </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B17" s="112" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="108" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="107"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="107"/>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107"/>
-      <c r="J17" s="107"/>
-      <c r="K17" s="107"/>
-      <c r="L17" s="107"/>
-      <c r="M17" s="107"/>
-      <c r="N17" s="107"/>
-      <c r="O17" s="107"/>
-      <c r="P17" s="107"/>
-      <c r="Q17" s="107"/>
-      <c r="R17" s="107"/>
-      <c r="S17" s="107"/>
-      <c r="T17" s="107"/>
-      <c r="U17" s="107"/>
-      <c r="V17" s="107"/>
-      <c r="W17" s="107"/>
-      <c r="X17" s="107"/>
-      <c r="Y17" s="107"/>
-      <c r="Z17" s="107"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B18" s="112" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="108" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="107"/>
-      <c r="E18" s="107"/>
-      <c r="F18" s="107"/>
-      <c r="G18" s="107"/>
-      <c r="H18" s="107"/>
-      <c r="I18" s="107"/>
-      <c r="J18" s="107"/>
-      <c r="K18" s="107"/>
-      <c r="L18" s="107"/>
-      <c r="M18" s="107"/>
-      <c r="N18" s="107"/>
-      <c r="O18" s="107"/>
-      <c r="P18" s="107"/>
-      <c r="Q18" s="107"/>
-      <c r="R18" s="107"/>
-      <c r="S18" s="107"/>
-      <c r="T18" s="107"/>
-      <c r="U18" s="107"/>
-      <c r="V18" s="107"/>
-      <c r="W18" s="107"/>
-      <c r="X18" s="107"/>
-      <c r="Y18" s="107"/>
-      <c r="Z18" s="107"/>
-    </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B19" s="111" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="107"/>
-      <c r="H19" s="107"/>
-      <c r="I19" s="107"/>
-      <c r="J19" s="107"/>
-      <c r="K19" s="107"/>
-      <c r="L19" s="107"/>
-      <c r="M19" s="107"/>
-      <c r="N19" s="107"/>
-      <c r="O19" s="107"/>
-      <c r="P19" s="107"/>
-      <c r="Q19" s="107"/>
-      <c r="R19" s="107"/>
-      <c r="S19" s="107"/>
-      <c r="T19" s="107"/>
-      <c r="U19" s="107"/>
-      <c r="V19" s="107"/>
-      <c r="W19" s="107"/>
-      <c r="X19" s="107"/>
-      <c r="Y19" s="107"/>
-      <c r="Z19" s="107"/>
-    </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B20" s="113" t="s">
+      <c r="C20" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="108" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="107"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="107"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="107"/>
-      <c r="J20" s="107"/>
-      <c r="K20" s="107"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="107"/>
-      <c r="N20" s="107"/>
-      <c r="O20" s="107"/>
-      <c r="P20" s="107"/>
-      <c r="Q20" s="107"/>
-      <c r="R20" s="107"/>
-      <c r="S20" s="107"/>
-      <c r="T20" s="107"/>
-      <c r="U20" s="107"/>
-      <c r="V20" s="107"/>
-      <c r="W20" s="107"/>
-      <c r="X20" s="107"/>
-      <c r="Y20" s="107"/>
-      <c r="Z20" s="107"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="104"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="104"/>
+      <c r="L20" s="104"/>
+      <c r="M20" s="104"/>
+      <c r="N20" s="104"/>
+      <c r="O20" s="104"/>
+      <c r="P20" s="104"/>
+      <c r="Q20" s="104"/>
+      <c r="R20" s="104"/>
+      <c r="S20" s="104"/>
+      <c r="T20" s="104"/>
+      <c r="U20" s="104"/>
+      <c r="V20" s="104"/>
+      <c r="W20" s="104"/>
+      <c r="X20" s="104"/>
+      <c r="Y20" s="104"/>
+      <c r="Z20" s="104"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B21" s="111" t="s">
+      <c r="A21" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21" s="108" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="105" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="104"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="104"/>
+      <c r="I21" s="104"/>
+      <c r="J21" s="104"/>
+      <c r="K21" s="104"/>
+      <c r="L21" s="104"/>
+      <c r="M21" s="104"/>
+      <c r="N21" s="104"/>
+      <c r="O21" s="104"/>
+      <c r="P21" s="104"/>
+      <c r="Q21" s="104"/>
+      <c r="R21" s="104"/>
+      <c r="S21" s="104"/>
+      <c r="T21" s="104"/>
+      <c r="U21" s="104"/>
+      <c r="V21" s="104"/>
+      <c r="W21" s="104"/>
+      <c r="X21" s="104"/>
+      <c r="Y21" s="104"/>
+      <c r="Z21" s="104"/>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B22" s="110" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="108" t="s">
-        <v>192</v>
-      </c>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="107"/>
-      <c r="K21" s="107"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="107"/>
-      <c r="N21" s="107"/>
-      <c r="O21" s="107"/>
-      <c r="P21" s="107"/>
-      <c r="Q21" s="107"/>
-      <c r="R21" s="107"/>
-      <c r="S21" s="107"/>
-      <c r="T21" s="107"/>
-      <c r="U21" s="107"/>
-      <c r="V21" s="107"/>
-      <c r="W21" s="107"/>
-      <c r="X21" s="107"/>
-      <c r="Y21" s="107"/>
-      <c r="Z21" s="107"/>
-    </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B22" s="113" t="s">
+      <c r="C22" s="105" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="108" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="107"/>
-      <c r="E22" s="107"/>
-      <c r="F22" s="107"/>
-      <c r="G22" s="107"/>
-      <c r="H22" s="107"/>
-      <c r="I22" s="107"/>
-      <c r="J22" s="107"/>
-      <c r="K22" s="107"/>
-      <c r="L22" s="107"/>
-      <c r="M22" s="107"/>
-      <c r="N22" s="107"/>
-      <c r="O22" s="107"/>
-      <c r="P22" s="107"/>
-      <c r="Q22" s="107"/>
-      <c r="R22" s="107"/>
-      <c r="S22" s="107"/>
-      <c r="T22" s="107"/>
-      <c r="U22" s="107"/>
-      <c r="V22" s="107"/>
-      <c r="W22" s="107"/>
-      <c r="X22" s="107"/>
-      <c r="Y22" s="107"/>
-      <c r="Z22" s="107"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="104"/>
+      <c r="I22" s="104"/>
+      <c r="J22" s="104"/>
+      <c r="K22" s="104"/>
+      <c r="L22" s="104"/>
+      <c r="M22" s="104"/>
+      <c r="N22" s="104"/>
+      <c r="O22" s="104"/>
+      <c r="P22" s="104"/>
+      <c r="Q22" s="104"/>
+      <c r="R22" s="104"/>
+      <c r="S22" s="104"/>
+      <c r="T22" s="104"/>
+      <c r="U22" s="104"/>
+      <c r="V22" s="104"/>
+      <c r="W22" s="104"/>
+      <c r="X22" s="104"/>
+      <c r="Y22" s="104"/>
+      <c r="Z22" s="104"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B23" s="111" t="s">
+      <c r="A23" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="108" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="105" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="108" t="s">
+      <c r="D23" s="104"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="104"/>
+      <c r="I23" s="104"/>
+      <c r="J23" s="104"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="104"/>
+      <c r="M23" s="104"/>
+      <c r="N23" s="104"/>
+      <c r="O23" s="104"/>
+      <c r="P23" s="104"/>
+      <c r="Q23" s="104"/>
+      <c r="R23" s="104"/>
+      <c r="S23" s="104"/>
+      <c r="T23" s="104"/>
+      <c r="U23" s="104"/>
+      <c r="V23" s="104"/>
+      <c r="W23" s="104"/>
+      <c r="X23" s="104"/>
+      <c r="Y23" s="104"/>
+      <c r="Z23" s="104"/>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="110" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="107"/>
-      <c r="E23" s="107"/>
-      <c r="F23" s="107"/>
-      <c r="G23" s="107"/>
-      <c r="H23" s="107"/>
-      <c r="I23" s="107"/>
-      <c r="J23" s="107"/>
-      <c r="K23" s="107"/>
-      <c r="L23" s="107"/>
-      <c r="M23" s="107"/>
-      <c r="N23" s="107"/>
-      <c r="O23" s="107"/>
-      <c r="P23" s="107"/>
-      <c r="Q23" s="107"/>
-      <c r="R23" s="107"/>
-      <c r="S23" s="107"/>
-      <c r="T23" s="107"/>
-      <c r="U23" s="107"/>
-      <c r="V23" s="107"/>
-      <c r="W23" s="107"/>
-      <c r="X23" s="107"/>
-      <c r="Y23" s="107"/>
-      <c r="Z23" s="107"/>
-    </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B24" s="113" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="108" t="s">
+      <c r="C24" s="105" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="104"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="104"/>
+      <c r="I24" s="104"/>
+      <c r="J24" s="104"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
+      <c r="M24" s="104"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="104"/>
+      <c r="P24" s="104"/>
+      <c r="Q24" s="104"/>
+      <c r="R24" s="104"/>
+      <c r="S24" s="104"/>
+      <c r="T24" s="104"/>
+      <c r="U24" s="104"/>
+      <c r="V24" s="104"/>
+      <c r="W24" s="104"/>
+      <c r="X24" s="104"/>
+      <c r="Y24" s="104"/>
+      <c r="Z24" s="104"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B25" s="108" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="105" t="s">
         <v>200</v>
       </c>
-      <c r="D24" s="107"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
-      <c r="G24" s="107"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="107"/>
-      <c r="J24" s="107"/>
-      <c r="K24" s="107"/>
-      <c r="L24" s="107"/>
-      <c r="M24" s="107"/>
-      <c r="N24" s="107"/>
-      <c r="O24" s="107"/>
-      <c r="P24" s="107"/>
-      <c r="Q24" s="107"/>
-      <c r="R24" s="107"/>
-      <c r="S24" s="107"/>
-      <c r="T24" s="107"/>
-      <c r="U24" s="107"/>
-      <c r="V24" s="107"/>
-      <c r="W24" s="107"/>
-      <c r="X24" s="107"/>
-      <c r="Y24" s="107"/>
-      <c r="Z24" s="107"/>
-    </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" s="111" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="108" t="s">
-        <v>201</v>
-      </c>
-      <c r="D25" s="107"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="107"/>
-      <c r="G25" s="107"/>
-      <c r="H25" s="107"/>
-      <c r="I25" s="107"/>
-      <c r="J25" s="107"/>
-      <c r="K25" s="107"/>
-      <c r="L25" s="107"/>
-      <c r="M25" s="107"/>
-      <c r="N25" s="107"/>
-      <c r="O25" s="107"/>
-      <c r="P25" s="107"/>
-      <c r="Q25" s="107"/>
-      <c r="R25" s="107"/>
-      <c r="S25" s="107"/>
-      <c r="T25" s="107"/>
-      <c r="U25" s="107"/>
-      <c r="V25" s="107"/>
-      <c r="W25" s="107"/>
-      <c r="X25" s="107"/>
-      <c r="Y25" s="107"/>
-      <c r="Z25" s="107"/>
+      <c r="D25" s="104"/>
+      <c r="E25" s="104"/>
+      <c r="F25" s="104"/>
+      <c r="G25" s="104"/>
+      <c r="H25" s="104"/>
+      <c r="I25" s="104"/>
+      <c r="J25" s="104"/>
+      <c r="K25" s="104"/>
+      <c r="L25" s="104"/>
+      <c r="M25" s="104"/>
+      <c r="N25" s="104"/>
+      <c r="O25" s="104"/>
+      <c r="P25" s="104"/>
+      <c r="Q25" s="104"/>
+      <c r="R25" s="104"/>
+      <c r="S25" s="104"/>
+      <c r="T25" s="104"/>
+      <c r="U25" s="104"/>
+      <c r="V25" s="104"/>
+      <c r="W25" s="104"/>
+      <c r="X25" s="104"/>
+      <c r="Y25" s="104"/>
+      <c r="Z25" s="104"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B26" s="111" t="s">
+      <c r="A26" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B26" s="108" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="108" t="s">
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="104"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="104"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="104"/>
+      <c r="L26" s="104"/>
+      <c r="M26" s="104"/>
+      <c r="N26" s="104"/>
+      <c r="O26" s="104"/>
+      <c r="P26" s="104"/>
+      <c r="Q26" s="104"/>
+      <c r="R26" s="104"/>
+      <c r="S26" s="104"/>
+      <c r="T26" s="104"/>
+      <c r="U26" s="104"/>
+      <c r="V26" s="104"/>
+      <c r="W26" s="104"/>
+      <c r="X26" s="104"/>
+      <c r="Y26" s="104"/>
+      <c r="Z26" s="104"/>
+    </row>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" s="108" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="107"/>
-      <c r="H26" s="107"/>
-      <c r="I26" s="107"/>
-      <c r="J26" s="107"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="107"/>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="107"/>
-      <c r="S26" s="107"/>
-      <c r="T26" s="107"/>
-      <c r="U26" s="107"/>
-      <c r="V26" s="107"/>
-      <c r="W26" s="107"/>
-      <c r="X26" s="107"/>
-      <c r="Y26" s="107"/>
-      <c r="Z26" s="107"/>
-    </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B27" s="111" t="s">
+      <c r="C27" s="105" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="108" t="s">
+      <c r="D27" s="104"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="104"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="104"/>
+      <c r="M27" s="104"/>
+      <c r="N27" s="104"/>
+      <c r="O27" s="104"/>
+      <c r="P27" s="104"/>
+      <c r="Q27" s="104"/>
+      <c r="R27" s="104"/>
+      <c r="S27" s="104"/>
+      <c r="T27" s="104"/>
+      <c r="U27" s="104"/>
+      <c r="V27" s="104"/>
+      <c r="W27" s="104"/>
+      <c r="X27" s="104"/>
+      <c r="Y27" s="104"/>
+      <c r="Z27" s="104"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B28" s="108" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="107"/>
-      <c r="I27" s="107"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="107"/>
-      <c r="L27" s="107"/>
-      <c r="M27" s="107"/>
-      <c r="N27" s="107"/>
-      <c r="O27" s="107"/>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="107"/>
-      <c r="S27" s="107"/>
-      <c r="T27" s="107"/>
-      <c r="U27" s="107"/>
-      <c r="V27" s="107"/>
-      <c r="W27" s="107"/>
-      <c r="X27" s="107"/>
-      <c r="Y27" s="107"/>
-      <c r="Z27" s="107"/>
-    </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B28" s="111" t="s">
+      <c r="C28" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="108" t="s">
+      <c r="D28" s="104"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="104"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="104"/>
+      <c r="M28" s="104"/>
+      <c r="N28" s="104"/>
+      <c r="O28" s="104"/>
+      <c r="P28" s="104"/>
+      <c r="Q28" s="104"/>
+      <c r="R28" s="104"/>
+      <c r="S28" s="104"/>
+      <c r="T28" s="104"/>
+      <c r="U28" s="104"/>
+      <c r="V28" s="104"/>
+      <c r="W28" s="104"/>
+      <c r="X28" s="104"/>
+      <c r="Y28" s="104"/>
+      <c r="Z28" s="104"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="108" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="107"/>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="107"/>
-      <c r="L28" s="107"/>
-      <c r="M28" s="107"/>
-      <c r="N28" s="107"/>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="107"/>
-      <c r="T28" s="107"/>
-      <c r="U28" s="107"/>
-      <c r="V28" s="107"/>
-      <c r="W28" s="107"/>
-      <c r="X28" s="107"/>
-      <c r="Y28" s="107"/>
-      <c r="Z28" s="107"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B29" s="111" t="s">
+      <c r="C29" s="111" t="s">
         <v>105</v>
       </c>
-      <c r="C29" s="114" t="s">
+      <c r="D29" s="104"/>
+      <c r="E29" s="104"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="104"/>
+      <c r="I29" s="104"/>
+      <c r="J29" s="104"/>
+      <c r="K29" s="104"/>
+      <c r="L29" s="104"/>
+      <c r="M29" s="104"/>
+      <c r="N29" s="104"/>
+      <c r="O29" s="104"/>
+      <c r="P29" s="104"/>
+      <c r="Q29" s="104"/>
+      <c r="R29" s="104"/>
+      <c r="S29" s="104"/>
+      <c r="T29" s="104"/>
+      <c r="U29" s="104"/>
+      <c r="V29" s="104"/>
+      <c r="W29" s="104"/>
+      <c r="X29" s="104"/>
+      <c r="Y29" s="104"/>
+      <c r="Z29" s="104"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="106" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="108" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" s="112" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="107"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="107"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="107"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-      <c r="S29" s="107"/>
-      <c r="T29" s="107"/>
-      <c r="U29" s="107"/>
-      <c r="V29" s="107"/>
-      <c r="W29" s="107"/>
-      <c r="X29" s="107"/>
-      <c r="Y29" s="107"/>
-      <c r="Z29" s="107"/>
-    </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="109" t="s">
-        <v>197</v>
-      </c>
-      <c r="B30" s="111" t="s">
+      <c r="D30" s="107"/>
+      <c r="E30" s="107"/>
+      <c r="F30" s="107"/>
+      <c r="G30" s="107"/>
+      <c r="H30" s="107"/>
+      <c r="I30" s="107"/>
+      <c r="J30" s="107"/>
+      <c r="K30" s="107"/>
+      <c r="L30" s="107"/>
+      <c r="M30" s="107"/>
+      <c r="N30" s="107"/>
+      <c r="O30" s="107"/>
+      <c r="P30" s="107"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="107"/>
+      <c r="S30" s="107"/>
+      <c r="T30" s="107"/>
+      <c r="U30" s="107"/>
+      <c r="V30" s="107"/>
+      <c r="W30" s="107"/>
+      <c r="X30" s="107"/>
+      <c r="Y30" s="107"/>
+      <c r="Z30" s="107"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" s="108" t="s">
         <v>150</v>
       </c>
-      <c r="C30" s="115" t="s">
+      <c r="C31" s="112" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="110"/>
-      <c r="E30" s="110"/>
-      <c r="F30" s="110"/>
-      <c r="G30" s="110"/>
-      <c r="H30" s="110"/>
-      <c r="I30" s="110"/>
-      <c r="J30" s="110"/>
-      <c r="K30" s="110"/>
-      <c r="L30" s="110"/>
-      <c r="M30" s="110"/>
-      <c r="N30" s="110"/>
-      <c r="O30" s="110"/>
-      <c r="P30" s="110"/>
-      <c r="Q30" s="110"/>
-      <c r="R30" s="110"/>
-      <c r="S30" s="110"/>
-      <c r="T30" s="110"/>
-      <c r="U30" s="110"/>
-      <c r="V30" s="110"/>
-      <c r="W30" s="110"/>
-      <c r="X30" s="110"/>
-      <c r="Y30" s="110"/>
-      <c r="Z30" s="110"/>
-    </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B31" s="111" t="s">
+      <c r="D31" s="104"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
+      <c r="K31" s="104"/>
+      <c r="L31" s="104"/>
+      <c r="M31" s="104"/>
+      <c r="N31" s="104"/>
+      <c r="O31" s="104"/>
+      <c r="P31" s="104"/>
+      <c r="Q31" s="104"/>
+      <c r="R31" s="104"/>
+      <c r="S31" s="104"/>
+      <c r="T31" s="104"/>
+      <c r="U31" s="104"/>
+      <c r="V31" s="104"/>
+      <c r="W31" s="104"/>
+      <c r="X31" s="104"/>
+      <c r="Y31" s="104"/>
+      <c r="Z31" s="104"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B32" s="108" t="s">
         <v>151</v>
       </c>
-      <c r="C31" s="115" t="s">
+      <c r="C32" s="112" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="107"/>
-      <c r="E31" s="107"/>
-      <c r="F31" s="107"/>
-      <c r="G31" s="107"/>
-      <c r="H31" s="107"/>
-      <c r="I31" s="107"/>
-      <c r="J31" s="107"/>
-      <c r="K31" s="107"/>
-      <c r="L31" s="107"/>
-      <c r="M31" s="107"/>
-      <c r="N31" s="107"/>
-      <c r="O31" s="107"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
-      <c r="S31" s="107"/>
-      <c r="T31" s="107"/>
-      <c r="U31" s="107"/>
-      <c r="V31" s="107"/>
-      <c r="W31" s="107"/>
-      <c r="X31" s="107"/>
-      <c r="Y31" s="107"/>
-      <c r="Z31" s="107"/>
-    </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B32" s="111" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" s="115" t="s">
+      <c r="D32" s="104"/>
+      <c r="E32" s="104"/>
+      <c r="F32" s="104"/>
+      <c r="G32" s="104"/>
+      <c r="H32" s="104"/>
+      <c r="I32" s="104"/>
+      <c r="J32" s="104"/>
+      <c r="K32" s="104"/>
+      <c r="L32" s="104"/>
+      <c r="M32" s="104"/>
+      <c r="N32" s="104"/>
+      <c r="O32" s="104"/>
+      <c r="P32" s="104"/>
+      <c r="Q32" s="104"/>
+      <c r="R32" s="104"/>
+      <c r="S32" s="104"/>
+      <c r="T32" s="104"/>
+      <c r="U32" s="104"/>
+      <c r="V32" s="104"/>
+      <c r="W32" s="104"/>
+      <c r="X32" s="104"/>
+      <c r="Y32" s="104"/>
+      <c r="Z32" s="104"/>
+    </row>
+    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="102" t="s">
+        <v>196</v>
+      </c>
+      <c r="B33" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="107"/>
-      <c r="E32" s="107"/>
-      <c r="F32" s="107"/>
-      <c r="G32" s="107"/>
-      <c r="H32" s="107"/>
-      <c r="I32" s="107"/>
-      <c r="J32" s="107"/>
-      <c r="K32" s="107"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="107"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="107"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="107"/>
-      <c r="R32" s="107"/>
-      <c r="S32" s="107"/>
-      <c r="T32" s="107"/>
-      <c r="U32" s="107"/>
-      <c r="V32" s="107"/>
-      <c r="W32" s="107"/>
-      <c r="X32" s="107"/>
-      <c r="Y32" s="107"/>
-      <c r="Z32" s="107"/>
-    </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B33" s="111" t="s">
+      <c r="C33" s="105" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="108" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="107"/>
-      <c r="E33" s="107"/>
-      <c r="F33" s="107"/>
-      <c r="G33" s="107"/>
-      <c r="H33" s="107"/>
-      <c r="I33" s="107"/>
-      <c r="J33" s="107"/>
-      <c r="K33" s="107"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="107"/>
-      <c r="N33" s="107"/>
-      <c r="O33" s="107"/>
-      <c r="P33" s="107"/>
-      <c r="Q33" s="107"/>
-      <c r="R33" s="107"/>
-      <c r="S33" s="107"/>
-      <c r="T33" s="107"/>
-      <c r="U33" s="107"/>
-      <c r="V33" s="107"/>
-      <c r="W33" s="107"/>
-      <c r="X33" s="107"/>
-      <c r="Y33" s="107"/>
-      <c r="Z33" s="107"/>
+      <c r="D33" s="104"/>
+      <c r="E33" s="104"/>
+      <c r="F33" s="104"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="104"/>
+      <c r="I33" s="104"/>
+      <c r="J33" s="104"/>
+      <c r="K33" s="104"/>
+      <c r="L33" s="104"/>
+      <c r="M33" s="104"/>
+      <c r="N33" s="104"/>
+      <c r="O33" s="104"/>
+      <c r="P33" s="104"/>
+      <c r="Q33" s="104"/>
+      <c r="R33" s="104"/>
+      <c r="S33" s="104"/>
+      <c r="T33" s="104"/>
+      <c r="U33" s="104"/>
+      <c r="V33" s="104"/>
+      <c r="W33" s="104"/>
+      <c r="X33" s="104"/>
+      <c r="Y33" s="104"/>
+      <c r="Z33" s="104"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>